<commit_message>
Debug incorrect variable name
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Urban\NCCS\nccs-nptrends\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpoongundranar\Documents\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AF2670-C186-4C80-9DE0-A6B4B6051E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A9ED6-04BA-45F4-81A8-F5AC4BF44BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary" sheetId="2" r:id="rId1"/>
@@ -2516,9 +2516,6 @@
     <t>CEOgender_specify</t>
   </si>
   <si>
-    <t>_12=estso</t>
-  </si>
-  <si>
     <t>BChairrace_AAPI</t>
   </si>
   <si>
@@ -3558,6 +3555,9 @@
   </si>
   <si>
     <t>Contact Information</t>
+  </si>
+  <si>
+    <t>FinanceChng_DcrsExp</t>
   </si>
 </sst>
 </file>
@@ -4014,8 +4014,8 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D169" sqref="D169"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4178,7 +4178,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -4450,19 +4450,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C20" t="s">
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F20" t="s">
         <v>597</v>
       </c>
       <c r="G20" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I20" t="s">
         <v>40</v>
@@ -4482,19 +4482,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F21" t="s">
         <v>597</v>
       </c>
       <c r="G21" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I21" t="s">
         <v>43</v>
@@ -4514,19 +4514,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F22" t="s">
         <v>597</v>
       </c>
       <c r="G22" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I22" t="s">
         <v>46</v>
@@ -4546,19 +4546,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F23" t="s">
         <v>597</v>
       </c>
       <c r="G23" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I23" t="s">
         <v>49</v>
@@ -4584,7 +4584,7 @@
         <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="E24" t="s">
         <v>677</v>
@@ -4593,7 +4593,7 @@
         <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="I24" t="s">
         <v>53</v>
@@ -4622,7 +4622,7 @@
         <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E25" t="s">
         <v>677</v>
@@ -4631,7 +4631,7 @@
         <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="I25" t="s">
         <v>56</v>
@@ -4654,19 +4654,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F26" t="s">
         <v>598</v>
       </c>
       <c r="G26" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I26" t="s">
         <v>40</v>
@@ -4686,19 +4686,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C27" t="s">
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F27" t="s">
         <v>598</v>
       </c>
       <c r="G27" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I27" t="s">
         <v>43</v>
@@ -4718,19 +4718,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C28" t="s">
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F28" t="s">
         <v>598</v>
       </c>
       <c r="G28" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I28" t="s">
         <v>46</v>
@@ -4750,19 +4750,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F29" t="s">
         <v>598</v>
       </c>
       <c r="G29" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I29" t="s">
         <v>49</v>
@@ -4782,13 +4782,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C30" t="s">
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E30" t="s">
         <v>677</v>
@@ -4820,13 +4820,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C31" t="s">
         <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E31" t="s">
         <v>677</v>
@@ -4864,7 +4864,7 @@
         <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E32" t="s">
         <v>677</v>
@@ -4902,16 +4902,16 @@
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F33" t="s">
         <v>600</v>
       </c>
       <c r="G33" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H33" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I33" t="s">
         <v>74</v>
@@ -4931,34 +4931,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C34" t="s">
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F34" t="s">
         <v>600</v>
       </c>
       <c r="G34" t="s">
+        <v>950</v>
+      </c>
+      <c r="H34" t="s">
         <v>951</v>
       </c>
-      <c r="H34" t="s">
-        <v>952</v>
-      </c>
       <c r="I34" t="s">
+        <v>994</v>
+      </c>
+      <c r="K34" t="s">
         <v>995</v>
-      </c>
-      <c r="K34" t="s">
-        <v>996</v>
       </c>
       <c r="L34" t="s">
         <v>73</v>
       </c>
       <c r="M34" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -4972,16 +4972,16 @@
         <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F35" t="s">
         <v>600</v>
       </c>
       <c r="G35" t="s">
+        <v>952</v>
+      </c>
+      <c r="H35" t="s">
         <v>953</v>
-      </c>
-      <c r="H35" t="s">
-        <v>954</v>
       </c>
       <c r="I35" t="s">
         <v>78</v>
@@ -5001,22 +5001,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C36" t="s">
         <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F36" t="s">
         <v>600</v>
       </c>
       <c r="G36" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H36" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I36" t="s">
         <v>81</v>
@@ -5036,34 +5036,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C37" t="s">
         <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F37" t="s">
         <v>600</v>
       </c>
       <c r="G37" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H37" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I37" t="s">
+        <v>996</v>
+      </c>
+      <c r="K37" t="s">
         <v>997</v>
-      </c>
-      <c r="K37" t="s">
-        <v>998</v>
       </c>
       <c r="L37" t="s">
         <v>73</v>
       </c>
       <c r="M37" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -5071,22 +5071,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C38" t="s">
         <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F38" t="s">
         <v>600</v>
       </c>
       <c r="G38" t="s">
+        <v>955</v>
+      </c>
+      <c r="H38" t="s">
         <v>956</v>
-      </c>
-      <c r="H38" t="s">
-        <v>957</v>
       </c>
       <c r="I38" t="s">
         <v>85</v>
@@ -5106,22 +5106,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C39" t="s">
         <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F39" t="s">
         <v>600</v>
       </c>
       <c r="G39" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H39" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I39" t="s">
         <v>88</v>
@@ -5141,22 +5141,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F40" t="s">
         <v>600</v>
       </c>
       <c r="G40" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="H40" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I40" t="s">
         <v>91</v>
@@ -5176,34 +5176,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C41" t="s">
         <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F41" t="s">
         <v>600</v>
       </c>
       <c r="G41" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="H41" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I41" t="s">
+        <v>999</v>
+      </c>
+      <c r="K41" t="s">
         <v>1000</v>
-      </c>
-      <c r="K41" t="s">
-        <v>1001</v>
       </c>
       <c r="L41" t="s">
         <v>73</v>
       </c>
       <c r="M41" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -5211,22 +5211,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C42" t="s">
         <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F42" t="s">
         <v>600</v>
       </c>
       <c r="G42" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="H42" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I42" t="s">
         <v>95</v>
@@ -5246,34 +5246,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C43" t="s">
         <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F43" t="s">
         <v>600</v>
       </c>
       <c r="G43" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="H43" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I43" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K43" t="s">
         <v>1003</v>
-      </c>
-      <c r="K43" t="s">
-        <v>1004</v>
       </c>
       <c r="L43" t="s">
         <v>73</v>
       </c>
       <c r="M43" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -5281,22 +5281,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C44" t="s">
         <v>97</v>
       </c>
       <c r="D44" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F44" t="s">
         <v>600</v>
       </c>
       <c r="G44" t="s">
+        <v>960</v>
+      </c>
+      <c r="H44" t="s">
         <v>961</v>
-      </c>
-      <c r="H44" t="s">
-        <v>962</v>
       </c>
       <c r="I44" t="s">
         <v>99</v>
@@ -5316,22 +5316,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C45" t="s">
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F45" t="s">
         <v>600</v>
       </c>
       <c r="G45" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="H45" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I45" t="s">
         <v>102</v>
@@ -5351,19 +5351,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C46" t="s">
         <v>103</v>
       </c>
       <c r="D46" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="F46" t="s">
         <v>600</v>
       </c>
       <c r="G46" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I46" t="s">
         <v>105</v>
@@ -5389,13 +5389,13 @@
         <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F47" t="s">
         <v>600</v>
       </c>
       <c r="G47" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I47" t="s">
         <v>108</v>
@@ -5421,16 +5421,16 @@
         <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F48" t="s">
         <v>601</v>
       </c>
       <c r="G48" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H48" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I48" t="s">
         <v>625</v>
@@ -5450,22 +5450,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C49" t="s">
         <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F49" t="s">
         <v>601</v>
       </c>
       <c r="G49" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H49" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I49" t="s">
         <v>626</v>
@@ -5485,22 +5485,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C50" t="s">
         <v>116</v>
       </c>
       <c r="D50" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F50" t="s">
         <v>602</v>
       </c>
       <c r="G50" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H50" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I50" t="s">
         <v>625</v>
@@ -5520,22 +5520,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C51" t="s">
         <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F51" t="s">
         <v>602</v>
       </c>
       <c r="G51" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H51" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I51" t="s">
         <v>627</v>
@@ -5561,10 +5561,10 @@
         <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="G52" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="K52" t="s">
         <v>123</v>
@@ -5587,13 +5587,13 @@
         <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F53" t="s">
         <v>603</v>
       </c>
       <c r="G53" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H53">
         <v>2021</v>
@@ -5622,13 +5622,13 @@
         <v>128</v>
       </c>
       <c r="D54" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F54" t="s">
         <v>603</v>
       </c>
       <c r="G54" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H54">
         <v>2021</v>
@@ -5657,13 +5657,13 @@
         <v>131</v>
       </c>
       <c r="D55" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F55" t="s">
         <v>603</v>
       </c>
       <c r="G55" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H55">
         <v>2021</v>
@@ -5692,13 +5692,13 @@
         <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F56" t="s">
         <v>603</v>
       </c>
       <c r="G56" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H56">
         <v>2021</v>
@@ -5727,13 +5727,13 @@
         <v>137</v>
       </c>
       <c r="D57" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F57" t="s">
         <v>603</v>
       </c>
       <c r="G57" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H57">
         <v>2021</v>
@@ -5762,13 +5762,13 @@
         <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F58" t="s">
         <v>603</v>
       </c>
       <c r="G58" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H58">
         <v>2021</v>
@@ -5797,13 +5797,13 @@
         <v>143</v>
       </c>
       <c r="D59" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F59" t="s">
         <v>603</v>
       </c>
       <c r="G59" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H59">
         <v>2021</v>
@@ -5832,7 +5832,7 @@
         <v>146</v>
       </c>
       <c r="D60" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F60" t="s">
         <v>603</v>
@@ -5867,7 +5867,7 @@
         <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F61" t="s">
         <v>603</v>
@@ -5902,13 +5902,13 @@
         <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F62" t="s">
         <v>604</v>
       </c>
       <c r="G62" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H62">
         <v>2022</v>
@@ -5937,13 +5937,13 @@
         <v>155</v>
       </c>
       <c r="D63" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F63" t="s">
         <v>604</v>
       </c>
       <c r="G63" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H63">
         <v>2022</v>
@@ -5972,13 +5972,13 @@
         <v>158</v>
       </c>
       <c r="D64" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F64" t="s">
         <v>604</v>
       </c>
       <c r="G64" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H64">
         <v>2022</v>
@@ -6007,13 +6007,13 @@
         <v>161</v>
       </c>
       <c r="D65" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F65" t="s">
         <v>604</v>
       </c>
       <c r="G65" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H65">
         <v>2022</v>
@@ -6042,13 +6042,13 @@
         <v>164</v>
       </c>
       <c r="D66" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F66" t="s">
         <v>604</v>
       </c>
       <c r="G66" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H66">
         <v>2022</v>
@@ -6077,13 +6077,13 @@
         <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F67" t="s">
         <v>604</v>
       </c>
       <c r="G67" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H67">
         <v>2022</v>
@@ -6112,13 +6112,13 @@
         <v>170</v>
       </c>
       <c r="D68" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F68" t="s">
         <v>604</v>
       </c>
       <c r="G68" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H68">
         <v>2022</v>
@@ -6147,7 +6147,7 @@
         <v>173</v>
       </c>
       <c r="D69" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F69" t="s">
         <v>604</v>
@@ -6182,7 +6182,7 @@
         <v>176</v>
       </c>
       <c r="D70" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F70" t="s">
         <v>604</v>
@@ -6217,13 +6217,13 @@
         <v>179</v>
       </c>
       <c r="D71" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F71" t="s">
         <v>605</v>
       </c>
       <c r="G71" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H71" t="s">
         <v>624</v>
@@ -6252,13 +6252,13 @@
         <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F72" t="s">
         <v>605</v>
       </c>
       <c r="G72" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H72" t="s">
         <v>624</v>
@@ -6287,13 +6287,13 @@
         <v>185</v>
       </c>
       <c r="D73" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F73" t="s">
         <v>605</v>
       </c>
       <c r="G73" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H73" t="s">
         <v>624</v>
@@ -6322,13 +6322,13 @@
         <v>188</v>
       </c>
       <c r="D74" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="F74" t="s">
         <v>605</v>
       </c>
       <c r="G74" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H74" t="s">
         <v>624</v>
@@ -6357,13 +6357,13 @@
         <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F75" t="s">
         <v>605</v>
       </c>
       <c r="G75" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H75" t="s">
         <v>624</v>
@@ -6392,13 +6392,13 @@
         <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F76" t="s">
         <v>605</v>
       </c>
       <c r="G76" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H76" t="s">
         <v>624</v>
@@ -6427,13 +6427,13 @@
         <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F77" t="s">
         <v>605</v>
       </c>
       <c r="G77" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H77" t="s">
         <v>624</v>
@@ -6462,7 +6462,7 @@
         <v>200</v>
       </c>
       <c r="D78" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F78" t="s">
         <v>605</v>
@@ -6497,7 +6497,7 @@
         <v>203</v>
       </c>
       <c r="D79" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F79" t="s">
         <v>605</v>
@@ -6532,7 +6532,7 @@
         <v>206</v>
       </c>
       <c r="D80" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="K80" t="s">
         <v>207</v>
@@ -6555,7 +6555,7 @@
         <v>208</v>
       </c>
       <c r="D81" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="K81" t="s">
         <v>209</v>
@@ -6578,16 +6578,16 @@
         <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="F82" t="s">
         <v>606</v>
       </c>
       <c r="G82" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H82" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I82" t="s">
         <v>213</v>
@@ -6613,16 +6613,16 @@
         <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F83" t="s">
         <v>606</v>
       </c>
       <c r="G83" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H83" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I83" t="s">
         <v>216</v>
@@ -6642,34 +6642,34 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C84" t="s">
         <v>217</v>
       </c>
       <c r="D84" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="F84" t="s">
         <v>606</v>
       </c>
       <c r="G84" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H84" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I84" t="s">
+        <v>1005</v>
+      </c>
+      <c r="K84" t="s">
         <v>1006</v>
-      </c>
-      <c r="K84" t="s">
-        <v>1007</v>
       </c>
       <c r="L84" t="s">
         <v>212</v>
       </c>
       <c r="M84" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -6683,16 +6683,16 @@
         <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="F85" t="s">
         <v>606</v>
       </c>
       <c r="G85" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H85" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I85" t="s">
         <v>220</v>
@@ -6712,34 +6712,34 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C86" t="s">
         <v>221</v>
       </c>
       <c r="D86" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="F86" t="s">
         <v>606</v>
       </c>
       <c r="G86" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H86" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I86" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K86" t="s">
         <v>1009</v>
-      </c>
-      <c r="K86" t="s">
-        <v>1010</v>
       </c>
       <c r="L86" t="s">
         <v>212</v>
       </c>
       <c r="M86" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -6753,16 +6753,16 @@
         <v>222</v>
       </c>
       <c r="D87" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F87" t="s">
         <v>606</v>
       </c>
       <c r="G87" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H87" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I87" t="s">
         <v>224</v>
@@ -6782,34 +6782,34 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C88" t="s">
         <v>225</v>
       </c>
       <c r="D88" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="F88" t="s">
         <v>606</v>
       </c>
       <c r="G88" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H88" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I88" t="s">
+        <v>1011</v>
+      </c>
+      <c r="K88" t="s">
         <v>1012</v>
-      </c>
-      <c r="K88" t="s">
-        <v>1013</v>
       </c>
       <c r="L88" t="s">
         <v>212</v>
       </c>
       <c r="M88" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -6823,16 +6823,16 @@
         <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F89" t="s">
         <v>606</v>
       </c>
       <c r="G89" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H89" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I89" t="s">
         <v>228</v>
@@ -6852,22 +6852,22 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C90" t="s">
         <v>229</v>
       </c>
       <c r="D90" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="F90" t="s">
         <v>606</v>
       </c>
       <c r="G90" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H90" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I90" t="s">
         <v>231</v>
@@ -6893,7 +6893,7 @@
         <v>232</v>
       </c>
       <c r="D91" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F91" t="s">
         <v>606</v>
@@ -6919,13 +6919,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C92" t="s">
         <v>235</v>
       </c>
       <c r="D92" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F92" t="s">
         <v>606</v>
@@ -6957,7 +6957,7 @@
         <v>238</v>
       </c>
       <c r="D93" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="K93" t="s">
         <v>239</v>
@@ -6980,16 +6980,16 @@
         <v>242</v>
       </c>
       <c r="D94" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F94" t="s">
         <v>607</v>
       </c>
       <c r="G94" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H94" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="I94" t="s">
         <v>652</v>
@@ -7015,16 +7015,16 @@
         <v>246</v>
       </c>
       <c r="D95" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F95" t="s">
         <v>607</v>
       </c>
       <c r="G95" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H95" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="I95" t="s">
         <v>653</v>
@@ -7050,16 +7050,16 @@
         <v>249</v>
       </c>
       <c r="D96" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F96" t="s">
         <v>607</v>
       </c>
       <c r="G96" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H96" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I96" t="s">
         <v>654</v>
@@ -7085,16 +7085,16 @@
         <v>252</v>
       </c>
       <c r="D97" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="F97" t="s">
         <v>607</v>
       </c>
       <c r="G97" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H97" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I97" t="s">
         <v>655</v>
@@ -7120,16 +7120,16 @@
         <v>255</v>
       </c>
       <c r="D98" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F98" t="s">
         <v>607</v>
       </c>
       <c r="G98" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H98" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I98" t="s">
         <v>656</v>
@@ -7155,16 +7155,16 @@
         <v>258</v>
       </c>
       <c r="D99" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F99" t="s">
         <v>607</v>
       </c>
       <c r="G99" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H99" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="I99" t="s">
         <v>657</v>
@@ -7190,16 +7190,16 @@
         <v>261</v>
       </c>
       <c r="D100" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F100" t="s">
         <v>607</v>
       </c>
       <c r="G100" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H100" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I100" t="s">
         <v>658</v>
@@ -7225,16 +7225,16 @@
         <v>264</v>
       </c>
       <c r="D101" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F101" t="s">
         <v>608</v>
       </c>
       <c r="G101" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H101" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="I101" t="s">
         <v>267</v>
@@ -7260,16 +7260,16 @@
         <v>268</v>
       </c>
       <c r="D102" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="F102" t="s">
         <v>608</v>
       </c>
       <c r="G102" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H102" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="I102" t="s">
         <v>270</v>
@@ -7295,7 +7295,7 @@
         <v>271</v>
       </c>
       <c r="D103" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F103" t="s">
         <v>609</v>
@@ -7333,7 +7333,7 @@
         <v>275</v>
       </c>
       <c r="D104" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F104" t="s">
         <v>609</v>
@@ -7342,7 +7342,7 @@
         <v>592</v>
       </c>
       <c r="H104" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I104" t="s">
         <v>660</v>
@@ -7371,7 +7371,7 @@
         <v>278</v>
       </c>
       <c r="D105" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F105" t="s">
         <v>609</v>
@@ -7380,7 +7380,7 @@
         <v>592</v>
       </c>
       <c r="H105" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I105" t="s">
         <v>661</v>
@@ -7406,7 +7406,7 @@
         <v>281</v>
       </c>
       <c r="D106" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="F106" t="s">
         <v>609</v>
@@ -7415,7 +7415,7 @@
         <v>592</v>
       </c>
       <c r="H106" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I106" t="s">
         <v>662</v>
@@ -7441,7 +7441,7 @@
         <v>284</v>
       </c>
       <c r="D107" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="F107" t="s">
         <v>609</v>
@@ -7450,7 +7450,7 @@
         <v>592</v>
       </c>
       <c r="H107" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I107" t="s">
         <v>663</v>
@@ -7476,7 +7476,7 @@
         <v>287</v>
       </c>
       <c r="D108" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F108" t="s">
         <v>609</v>
@@ -7485,7 +7485,7 @@
         <v>592</v>
       </c>
       <c r="H108" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I108" t="s">
         <v>664</v>
@@ -7511,7 +7511,7 @@
         <v>290</v>
       </c>
       <c r="D109" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F109" t="s">
         <v>609</v>
@@ -7520,7 +7520,7 @@
         <v>592</v>
       </c>
       <c r="H109" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I109" t="s">
         <v>665</v>
@@ -7546,7 +7546,7 @@
         <v>293</v>
       </c>
       <c r="D110" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F110" t="s">
         <v>609</v>
@@ -7555,7 +7555,7 @@
         <v>592</v>
       </c>
       <c r="H110" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I110" t="s">
         <v>666</v>
@@ -7581,7 +7581,7 @@
         <v>296</v>
       </c>
       <c r="D111" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F111" t="s">
         <v>609</v>
@@ -7590,7 +7590,7 @@
         <v>592</v>
       </c>
       <c r="H111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I111" t="s">
         <v>667</v>
@@ -7616,7 +7616,7 @@
         <v>299</v>
       </c>
       <c r="D112" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F112" t="s">
         <v>609</v>
@@ -7625,7 +7625,7 @@
         <v>592</v>
       </c>
       <c r="H112" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I112" t="s">
         <v>668</v>
@@ -7651,7 +7651,7 @@
         <v>302</v>
       </c>
       <c r="D113" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F113" t="s">
         <v>609</v>
@@ -7660,7 +7660,7 @@
         <v>592</v>
       </c>
       <c r="H113" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I113" t="s">
         <v>669</v>
@@ -7686,7 +7686,7 @@
         <v>305</v>
       </c>
       <c r="D114" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F114" t="s">
         <v>609</v>
@@ -7695,7 +7695,7 @@
         <v>592</v>
       </c>
       <c r="H114" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I114" t="s">
         <v>670</v>
@@ -7721,7 +7721,7 @@
         <v>308</v>
       </c>
       <c r="D115" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="F115" t="s">
         <v>609</v>
@@ -7730,7 +7730,7 @@
         <v>592</v>
       </c>
       <c r="H115" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I115" t="s">
         <v>671</v>
@@ -7756,7 +7756,7 @@
         <v>311</v>
       </c>
       <c r="D116" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="F116" t="s">
         <v>610</v>
@@ -7791,7 +7791,7 @@
         <v>314</v>
       </c>
       <c r="D117" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F117" t="s">
         <v>610</v>
@@ -7800,7 +7800,7 @@
         <v>593</v>
       </c>
       <c r="H117" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I117" t="s">
         <v>660</v>
@@ -7826,7 +7826,7 @@
         <v>317</v>
       </c>
       <c r="D118" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="F118" t="s">
         <v>610</v>
@@ -7835,7 +7835,7 @@
         <v>593</v>
       </c>
       <c r="H118" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I118" t="s">
         <v>661</v>
@@ -7861,7 +7861,7 @@
         <v>320</v>
       </c>
       <c r="D119" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F119" t="s">
         <v>610</v>
@@ -7870,7 +7870,7 @@
         <v>593</v>
       </c>
       <c r="H119" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I119" t="s">
         <v>662</v>
@@ -7896,7 +7896,7 @@
         <v>323</v>
       </c>
       <c r="D120" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="F120" t="s">
         <v>610</v>
@@ -7905,7 +7905,7 @@
         <v>593</v>
       </c>
       <c r="H120" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I120" t="s">
         <v>663</v>
@@ -7931,7 +7931,7 @@
         <v>326</v>
       </c>
       <c r="D121" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F121" t="s">
         <v>610</v>
@@ -7940,7 +7940,7 @@
         <v>593</v>
       </c>
       <c r="H121" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I121" t="s">
         <v>664</v>
@@ -7966,7 +7966,7 @@
         <v>329</v>
       </c>
       <c r="D122" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F122" t="s">
         <v>610</v>
@@ -7975,7 +7975,7 @@
         <v>593</v>
       </c>
       <c r="H122" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I122" t="s">
         <v>665</v>
@@ -8001,7 +8001,7 @@
         <v>332</v>
       </c>
       <c r="D123" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="F123" t="s">
         <v>610</v>
@@ -8010,7 +8010,7 @@
         <v>593</v>
       </c>
       <c r="H123" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I123" t="s">
         <v>666</v>
@@ -8036,7 +8036,7 @@
         <v>335</v>
       </c>
       <c r="D124" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="F124" t="s">
         <v>610</v>
@@ -8045,7 +8045,7 @@
         <v>593</v>
       </c>
       <c r="H124" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I124" t="s">
         <v>667</v>
@@ -8071,7 +8071,7 @@
         <v>338</v>
       </c>
       <c r="D125" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F125" t="s">
         <v>610</v>
@@ -8080,7 +8080,7 @@
         <v>593</v>
       </c>
       <c r="H125" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I125" t="s">
         <v>668</v>
@@ -8106,7 +8106,7 @@
         <v>341</v>
       </c>
       <c r="D126" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F126" t="s">
         <v>610</v>
@@ -8115,7 +8115,7 @@
         <v>593</v>
       </c>
       <c r="H126" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I126" t="s">
         <v>669</v>
@@ -8141,7 +8141,7 @@
         <v>344</v>
       </c>
       <c r="D127" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="F127" t="s">
         <v>610</v>
@@ -8150,7 +8150,7 @@
         <v>593</v>
       </c>
       <c r="H127" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I127" t="s">
         <v>670</v>
@@ -8176,7 +8176,7 @@
         <v>347</v>
       </c>
       <c r="D128" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="F128" t="s">
         <v>610</v>
@@ -8185,7 +8185,7 @@
         <v>593</v>
       </c>
       <c r="H128" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I128" t="s">
         <v>671</v>
@@ -8211,16 +8211,16 @@
         <v>350</v>
       </c>
       <c r="D129" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F129" t="s">
         <v>611</v>
       </c>
       <c r="G129" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H129" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I129" t="s">
         <v>353</v>
@@ -8249,16 +8249,16 @@
         <v>354</v>
       </c>
       <c r="D130" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F130" t="s">
         <v>611</v>
       </c>
       <c r="G130" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H130" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I130" t="s">
         <v>356</v>
@@ -8287,16 +8287,16 @@
         <v>357</v>
       </c>
       <c r="D131" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F131" t="s">
         <v>611</v>
       </c>
       <c r="G131" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H131" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="I131" t="s">
         <v>359</v>
@@ -8325,16 +8325,16 @@
         <v>360</v>
       </c>
       <c r="D132" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F132" t="s">
         <v>611</v>
       </c>
       <c r="G132" t="s">
+        <v>893</v>
+      </c>
+      <c r="H132" t="s">
         <v>894</v>
-      </c>
-      <c r="H132" t="s">
-        <v>895</v>
       </c>
       <c r="I132" t="s">
         <v>362</v>
@@ -8363,16 +8363,16 @@
         <v>363</v>
       </c>
       <c r="D133" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F133" t="s">
         <v>611</v>
       </c>
       <c r="G133" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H133" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I133" t="s">
         <v>365</v>
@@ -8401,16 +8401,16 @@
         <v>366</v>
       </c>
       <c r="D134" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="F134" t="s">
         <v>611</v>
       </c>
       <c r="G134" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H134" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I134" t="s">
         <v>368</v>
@@ -8439,16 +8439,16 @@
         <v>369</v>
       </c>
       <c r="D135" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F135" t="s">
         <v>611</v>
       </c>
       <c r="G135" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H135" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I135" t="s">
         <v>371</v>
@@ -8477,13 +8477,13 @@
         <v>372</v>
       </c>
       <c r="D136" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F136" t="s">
         <v>611</v>
       </c>
       <c r="G136" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H136" t="s">
         <v>623</v>
@@ -8515,13 +8515,13 @@
         <v>374</v>
       </c>
       <c r="D137" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F137" t="s">
         <v>611</v>
       </c>
       <c r="G137" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H137" t="s">
         <v>623</v>
@@ -8547,13 +8547,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C138" t="s">
         <v>376</v>
       </c>
       <c r="D138" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F138" t="s">
         <v>612</v>
@@ -8576,13 +8576,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C139" t="s">
         <v>377</v>
       </c>
       <c r="D139" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F139" t="s">
         <v>612</v>
@@ -8605,13 +8605,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C140" t="s">
         <v>378</v>
       </c>
       <c r="D140" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F140" t="s">
         <v>612</v>
@@ -8634,13 +8634,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C141" t="s">
         <v>379</v>
       </c>
       <c r="D141" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="F141" t="s">
         <v>612</v>
@@ -8669,16 +8669,16 @@
         <v>380</v>
       </c>
       <c r="D142" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E142" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F142" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G142" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="J142" s="2">
         <v>1</v>
@@ -8704,13 +8704,13 @@
         <v>384</v>
       </c>
       <c r="D143" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E143" t="s">
+        <v>898</v>
+      </c>
+      <c r="F143" t="s">
         <v>899</v>
-      </c>
-      <c r="F143" t="s">
-        <v>900</v>
       </c>
       <c r="K143" t="s">
         <v>385</v>
@@ -8733,13 +8733,13 @@
         <v>387</v>
       </c>
       <c r="D144" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F144" t="s">
+        <v>899</v>
+      </c>
+      <c r="G144" t="s">
         <v>900</v>
-      </c>
-      <c r="G144" t="s">
-        <v>901</v>
       </c>
       <c r="K144" t="s">
         <v>388</v>
@@ -8762,16 +8762,16 @@
         <v>389</v>
       </c>
       <c r="D145" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E145" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F145" t="s">
+        <v>899</v>
+      </c>
+      <c r="G145" t="s">
         <v>900</v>
-      </c>
-      <c r="G145" t="s">
-        <v>901</v>
       </c>
       <c r="J145" s="2">
         <v>1</v>
@@ -8797,13 +8797,13 @@
         <v>393</v>
       </c>
       <c r="D146" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F146" t="s">
         <v>613</v>
       </c>
       <c r="G146" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I146" t="s">
         <v>396</v>
@@ -8829,13 +8829,13 @@
         <v>397</v>
       </c>
       <c r="D147" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="F147" t="s">
         <v>613</v>
       </c>
       <c r="G147" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I147" t="s">
         <v>399</v>
@@ -8855,31 +8855,31 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C148" t="s">
         <v>400</v>
       </c>
       <c r="D148" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F148" t="s">
         <v>613</v>
       </c>
       <c r="G148" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I148" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K148" t="s">
         <v>1016</v>
-      </c>
-      <c r="K148" t="s">
-        <v>1017</v>
       </c>
       <c r="L148" t="s">
         <v>395</v>
       </c>
       <c r="M148" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.3">
@@ -8893,13 +8893,13 @@
         <v>401</v>
       </c>
       <c r="D149" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F149" t="s">
         <v>613</v>
       </c>
       <c r="G149" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I149" t="s">
         <v>403</v>
@@ -8925,13 +8925,13 @@
         <v>404</v>
       </c>
       <c r="D150" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F150" t="s">
         <v>613</v>
       </c>
       <c r="G150" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I150" t="s">
         <v>406</v>
@@ -8951,19 +8951,19 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1015</v>
+        <v>1169</v>
       </c>
       <c r="C151" t="s">
         <v>407</v>
       </c>
       <c r="D151" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F151" t="s">
         <v>613</v>
       </c>
       <c r="G151" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I151" t="s">
         <v>409</v>
@@ -8989,7 +8989,7 @@
         <v>410</v>
       </c>
       <c r="D152" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F152" t="s">
         <v>613</v>
@@ -9021,7 +9021,7 @@
         <v>412</v>
       </c>
       <c r="D153" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F153" t="s">
         <v>613</v>
@@ -9053,16 +9053,16 @@
         <v>414</v>
       </c>
       <c r="D154" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F154" t="s">
         <v>614</v>
       </c>
       <c r="G154" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H154" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I154" t="s">
         <v>417</v>
@@ -9088,16 +9088,16 @@
         <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="F155" t="s">
         <v>614</v>
       </c>
       <c r="G155" t="s">
+        <v>905</v>
+      </c>
+      <c r="H155" t="s">
         <v>906</v>
-      </c>
-      <c r="H155" t="s">
-        <v>907</v>
       </c>
       <c r="I155" t="s">
         <v>420</v>
@@ -9123,16 +9123,16 @@
         <v>421</v>
       </c>
       <c r="D156" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F156" t="s">
         <v>614</v>
       </c>
       <c r="G156" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H156" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I156" t="s">
         <v>423</v>
@@ -9158,16 +9158,16 @@
         <v>424</v>
       </c>
       <c r="D157" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F157" t="s">
         <v>614</v>
       </c>
       <c r="G157" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H157" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I157" t="s">
         <v>426</v>
@@ -9193,16 +9193,16 @@
         <v>427</v>
       </c>
       <c r="D158" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F158" t="s">
         <v>614</v>
       </c>
       <c r="G158" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H158" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I158" t="s">
         <v>429</v>
@@ -9228,16 +9228,16 @@
         <v>430</v>
       </c>
       <c r="D159" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F159" t="s">
         <v>614</v>
       </c>
       <c r="G159" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H159" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I159" t="s">
         <v>432</v>
@@ -9263,16 +9263,16 @@
         <v>433</v>
       </c>
       <c r="D160" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F160" t="s">
         <v>614</v>
       </c>
       <c r="G160" t="s">
+        <v>910</v>
+      </c>
+      <c r="H160" t="s">
         <v>911</v>
-      </c>
-      <c r="H160" t="s">
-        <v>912</v>
       </c>
       <c r="I160" t="s">
         <v>435</v>
@@ -9298,16 +9298,16 @@
         <v>436</v>
       </c>
       <c r="D161" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F161" t="s">
         <v>614</v>
       </c>
       <c r="G161" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H161" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I161" t="s">
         <v>438</v>
@@ -9333,16 +9333,16 @@
         <v>439</v>
       </c>
       <c r="D162" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="F162" t="s">
         <v>614</v>
       </c>
       <c r="G162" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H162" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="I162" t="s">
         <v>441</v>
@@ -9368,7 +9368,7 @@
         <v>442</v>
       </c>
       <c r="D163" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F163" t="s">
         <v>614</v>
@@ -9397,7 +9397,7 @@
         <v>444</v>
       </c>
       <c r="D164" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F164" t="s">
         <v>614</v>
@@ -9426,7 +9426,7 @@
         <v>446</v>
       </c>
       <c r="D165" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E165" t="s">
         <v>678</v>
@@ -9435,10 +9435,10 @@
         <v>615</v>
       </c>
       <c r="G165" t="s">
+        <v>914</v>
+      </c>
+      <c r="H165" t="s">
         <v>915</v>
-      </c>
-      <c r="H165" t="s">
-        <v>916</v>
       </c>
       <c r="I165" t="s">
         <v>449</v>
@@ -9464,7 +9464,7 @@
         <v>450</v>
       </c>
       <c r="D166" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E166" t="s">
         <v>678</v>
@@ -9473,10 +9473,10 @@
         <v>615</v>
       </c>
       <c r="G166" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H166" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I166" t="s">
         <v>452</v>
@@ -9502,7 +9502,7 @@
         <v>453</v>
       </c>
       <c r="D167" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E167" t="s">
         <v>678</v>
@@ -9511,10 +9511,10 @@
         <v>615</v>
       </c>
       <c r="G167" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H167" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I167" t="s">
         <v>455</v>
@@ -9540,7 +9540,7 @@
         <v>456</v>
       </c>
       <c r="D168" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E168" t="s">
         <v>678</v>
@@ -9549,10 +9549,10 @@
         <v>615</v>
       </c>
       <c r="G168" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H168" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I168" t="s">
         <v>458</v>
@@ -9578,7 +9578,7 @@
         <v>459</v>
       </c>
       <c r="D169" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E169" t="s">
         <v>678</v>
@@ -9587,10 +9587,10 @@
         <v>615</v>
       </c>
       <c r="G169" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H169" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I169" t="s">
         <v>461</v>
@@ -9616,7 +9616,7 @@
         <v>462</v>
       </c>
       <c r="D170" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E170" t="s">
         <v>678</v>
@@ -9625,7 +9625,7 @@
         <v>615</v>
       </c>
       <c r="G170" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H170" t="s">
         <v>623</v>
@@ -9654,7 +9654,7 @@
         <v>465</v>
       </c>
       <c r="D171" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E171" t="s">
         <v>678</v>
@@ -9663,7 +9663,7 @@
         <v>615</v>
       </c>
       <c r="G171" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H171" t="s">
         <v>623</v>
@@ -9692,7 +9692,7 @@
         <v>468</v>
       </c>
       <c r="D172" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E172" t="s">
         <v>678</v>
@@ -9701,10 +9701,10 @@
         <v>616</v>
       </c>
       <c r="G172" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H172" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I172" t="s">
         <v>471</v>
@@ -9730,7 +9730,7 @@
         <v>472</v>
       </c>
       <c r="D173" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E173" t="s">
         <v>678</v>
@@ -9739,10 +9739,10 @@
         <v>616</v>
       </c>
       <c r="G173" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H173" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I173" t="s">
         <v>474</v>
@@ -9768,7 +9768,7 @@
         <v>475</v>
       </c>
       <c r="D174" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E174" t="s">
         <v>678</v>
@@ -9777,10 +9777,10 @@
         <v>616</v>
       </c>
       <c r="G174" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H174" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I174" t="s">
         <v>477</v>
@@ -9806,7 +9806,7 @@
         <v>478</v>
       </c>
       <c r="D175" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E175" t="s">
         <v>678</v>
@@ -9815,10 +9815,10 @@
         <v>616</v>
       </c>
       <c r="G175" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H175" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I175" t="s">
         <v>480</v>
@@ -9844,7 +9844,7 @@
         <v>481</v>
       </c>
       <c r="D176" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E176" t="s">
         <v>678</v>
@@ -9853,7 +9853,7 @@
         <v>616</v>
       </c>
       <c r="G176" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H176" t="s">
         <v>623</v>
@@ -9882,7 +9882,7 @@
         <v>483</v>
       </c>
       <c r="D177" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E177" t="s">
         <v>678</v>
@@ -9891,7 +9891,7 @@
         <v>616</v>
       </c>
       <c r="G177" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H177" t="s">
         <v>623</v>
@@ -9914,13 +9914,13 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C178" t="s">
         <v>485</v>
       </c>
       <c r="D178" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E178" t="s">
         <v>678</v>
@@ -9929,10 +9929,10 @@
         <v>617</v>
       </c>
       <c r="G178" t="s">
+        <v>914</v>
+      </c>
+      <c r="H178" t="s">
         <v>915</v>
-      </c>
-      <c r="H178" t="s">
-        <v>916</v>
       </c>
       <c r="I178" t="s">
         <v>449</v>
@@ -9952,13 +9952,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C179" t="s">
         <v>488</v>
       </c>
       <c r="D179" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E179" t="s">
         <v>678</v>
@@ -9967,10 +9967,10 @@
         <v>617</v>
       </c>
       <c r="G179" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H179" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I179" t="s">
         <v>452</v>
@@ -9990,13 +9990,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C180" t="s">
         <v>490</v>
       </c>
       <c r="D180" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E180" t="s">
         <v>678</v>
@@ -10005,10 +10005,10 @@
         <v>617</v>
       </c>
       <c r="G180" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H180" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I180" t="s">
         <v>455</v>
@@ -10028,13 +10028,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C181" t="s">
         <v>492</v>
       </c>
       <c r="D181" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E181" t="s">
         <v>678</v>
@@ -10043,10 +10043,10 @@
         <v>617</v>
       </c>
       <c r="G181" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H181" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I181" t="s">
         <v>458</v>
@@ -10066,13 +10066,13 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C182" t="s">
         <v>494</v>
       </c>
       <c r="D182" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E182" t="s">
         <v>678</v>
@@ -10081,10 +10081,10 @@
         <v>617</v>
       </c>
       <c r="G182" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H182" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I182" t="s">
         <v>461</v>
@@ -10104,13 +10104,13 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C183" t="s">
         <v>496</v>
       </c>
       <c r="D183" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E183" t="s">
         <v>678</v>
@@ -10119,7 +10119,7 @@
         <v>617</v>
       </c>
       <c r="G183" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H183" t="s">
         <v>623</v>
@@ -10142,13 +10142,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C184" t="s">
         <v>498</v>
       </c>
       <c r="D184" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E184" t="s">
         <v>678</v>
@@ -10157,7 +10157,7 @@
         <v>617</v>
       </c>
       <c r="G184" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="H184" t="s">
         <v>623</v>
@@ -10180,13 +10180,13 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C185" t="s">
         <v>500</v>
       </c>
       <c r="D185" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E185" t="s">
         <v>678</v>
@@ -10195,10 +10195,10 @@
         <v>618</v>
       </c>
       <c r="G185" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H185" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I185" t="s">
         <v>503</v>
@@ -10218,13 +10218,13 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C186" t="s">
         <v>504</v>
       </c>
       <c r="D186" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E186" t="s">
         <v>678</v>
@@ -10233,10 +10233,10 @@
         <v>618</v>
       </c>
       <c r="G186" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H186" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I186" t="s">
         <v>506</v>
@@ -10256,13 +10256,13 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C187" t="s">
         <v>507</v>
       </c>
       <c r="D187" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E187" t="s">
         <v>678</v>
@@ -10271,10 +10271,10 @@
         <v>618</v>
       </c>
       <c r="G187" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H187" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I187" t="s">
         <v>477</v>
@@ -10294,13 +10294,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C188" t="s">
         <v>509</v>
       </c>
       <c r="D188" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E188" t="s">
         <v>678</v>
@@ -10309,10 +10309,10 @@
         <v>618</v>
       </c>
       <c r="G188" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H188" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I188" t="s">
         <v>480</v>
@@ -10332,13 +10332,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C189" t="s">
         <v>511</v>
       </c>
       <c r="D189" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E189" t="s">
         <v>678</v>
@@ -10347,7 +10347,7 @@
         <v>618</v>
       </c>
       <c r="G189" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H189" t="s">
         <v>623</v>
@@ -10370,13 +10370,13 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C190" t="s">
         <v>513</v>
       </c>
       <c r="D190" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E190" t="s">
         <v>678</v>
@@ -10385,7 +10385,7 @@
         <v>618</v>
       </c>
       <c r="G190" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H190" t="s">
         <v>623</v>
@@ -10408,22 +10408,22 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C191" t="s">
         <v>515</v>
       </c>
       <c r="D191" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E191" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F191" t="s">
         <v>619</v>
       </c>
       <c r="G191" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="I191" t="s">
         <v>518</v>
@@ -10443,22 +10443,22 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C192" t="s">
         <v>519</v>
       </c>
       <c r="D192" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E192" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F192" t="s">
         <v>619</v>
       </c>
       <c r="G192" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I192" t="s">
         <v>521</v>
@@ -10478,22 +10478,22 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C193" t="s">
         <v>522</v>
       </c>
       <c r="D193" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E193" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F193" t="s">
         <v>619</v>
       </c>
       <c r="G193" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I193" t="s">
         <v>524</v>
@@ -10513,22 +10513,22 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C194" t="s">
         <v>525</v>
       </c>
       <c r="D194" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E194" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F194" t="s">
         <v>619</v>
       </c>
       <c r="G194" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I194" t="s">
         <v>527</v>
@@ -10548,22 +10548,22 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C195" t="s">
         <v>528</v>
       </c>
       <c r="D195" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E195" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F195" t="s">
         <v>619</v>
       </c>
       <c r="G195" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I195" t="s">
         <v>530</v>
@@ -10583,22 +10583,22 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C196" t="s">
         <v>531</v>
       </c>
       <c r="D196" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E196" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F196" t="s">
         <v>619</v>
       </c>
       <c r="G196" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="I196" t="s">
         <v>533</v>
@@ -10618,22 +10618,22 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C197" t="s">
         <v>534</v>
       </c>
       <c r="D197" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E197" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F197" t="s">
         <v>619</v>
       </c>
       <c r="G197" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I197" t="s">
         <v>536</v>
@@ -10653,22 +10653,22 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C198" t="s">
         <v>537</v>
       </c>
       <c r="D198" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E198" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F198" t="s">
         <v>619</v>
       </c>
       <c r="G198" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I198" t="s">
         <v>539</v>
@@ -10688,22 +10688,22 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C199" t="s">
         <v>540</v>
       </c>
       <c r="D199" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E199" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F199" t="s">
         <v>619</v>
       </c>
       <c r="G199" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="I199" t="s">
         <v>542</v>
@@ -10723,22 +10723,22 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C200" t="s">
         <v>543</v>
       </c>
       <c r="D200" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E200" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F200" t="s">
         <v>619</v>
       </c>
       <c r="G200" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I200" t="s">
         <v>545</v>
@@ -10758,22 +10758,22 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C201" t="s">
         <v>546</v>
       </c>
       <c r="D201" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E201" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F201" t="s">
         <v>619</v>
       </c>
       <c r="G201" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I201" t="s">
         <v>548</v>
@@ -10793,22 +10793,22 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C202" t="s">
         <v>549</v>
       </c>
       <c r="D202" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E202" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F202" t="s">
         <v>619</v>
       </c>
       <c r="G202" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I202" t="s">
         <v>551</v>
@@ -10828,22 +10828,22 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C203" t="s">
         <v>552</v>
       </c>
       <c r="D203" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E203" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F203" t="s">
         <v>619</v>
       </c>
       <c r="G203" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I203" t="s">
         <v>554</v>
@@ -10863,13 +10863,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C204" t="s">
         <v>555</v>
       </c>
       <c r="D204" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K204" t="s">
         <v>556</v>
@@ -10906,7 +10906,7 @@
         <v>559</v>
       </c>
       <c r="D206" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F206" t="s">
         <v>620</v>
@@ -10935,7 +10935,7 @@
         <v>562</v>
       </c>
       <c r="D207" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F207" t="s">
         <v>620</v>
@@ -10964,7 +10964,7 @@
         <v>565</v>
       </c>
       <c r="D208" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F208" t="s">
         <v>620</v>
@@ -11013,7 +11013,7 @@
         <v>570</v>
       </c>
       <c r="D210" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="J210" s="2">
         <v>1</v>
@@ -11076,7 +11076,7 @@
         <v>573</v>
       </c>
       <c r="D213" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="J213" s="2">
         <v>1</v>
@@ -11119,7 +11119,7 @@
         <v>575</v>
       </c>
       <c r="D215" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="K215" t="s">
         <v>575</v>
@@ -11142,7 +11142,7 @@
         <v>576</v>
       </c>
       <c r="D216" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="K216" t="s">
         <v>576</v>
@@ -11216,13 +11216,13 @@
         <v>219</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>822</v>
+        <v>673</v>
       </c>
       <c r="C220" t="s">
-        <v>673</v>
+        <v>581</v>
       </c>
       <c r="D220" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="I220" t="s">
         <v>674</v>
@@ -11248,7 +11248,7 @@
         <v>582</v>
       </c>
       <c r="D221" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="J221" s="2">
         <v>1</v>
@@ -11271,7 +11271,7 @@
         <v>583</v>
       </c>
       <c r="D222" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="J222" s="2">
         <v>1</v>
@@ -11317,7 +11317,7 @@
         <v>585</v>
       </c>
       <c r="D224" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="J224" s="2">
         <v>1</v>
@@ -11340,7 +11340,7 @@
         <v>586</v>
       </c>
       <c r="D225" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="J225" s="2">
         <v>1</v>
@@ -11363,7 +11363,7 @@
         <v>587</v>
       </c>
       <c r="D226" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J226" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Fix incorrect variable name
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpoongundranar\Documents\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A9ED6-04BA-45F4-81A8-F5AC4BF44BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D50690-37DC-447D-92EF-AE0FDEC01453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary" sheetId="2" r:id="rId1"/>
@@ -2411,9 +2411,6 @@
     <t>Finance_Rev_Oth</t>
   </si>
   <si>
-    <t>Finance_Rev_Tot</t>
-  </si>
-  <si>
     <t>Reserves_Est</t>
   </si>
   <si>
@@ -3233,9 +3230,6 @@
     <t>total revenue from other sources</t>
   </si>
   <si>
-    <t>total revenue from all sources</t>
-  </si>
-  <si>
     <t>Time at which first click was recorded for finance questions</t>
   </si>
   <si>
@@ -3558,6 +3552,12 @@
   </si>
   <si>
     <t>FinanceChng_DcrsExp</t>
+  </si>
+  <si>
+    <t>Finance_Rev_Oth_Text</t>
+  </si>
+  <si>
+    <t>names of other revenue sources</t>
   </si>
 </sst>
 </file>
@@ -3715,9 +3715,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3755,7 +3755,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3861,7 +3861,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4003,7 +4003,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4014,8 +4014,8 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4178,7 +4178,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -4450,19 +4450,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C20" t="s">
         <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F20" t="s">
         <v>597</v>
       </c>
       <c r="G20" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I20" t="s">
         <v>40</v>
@@ -4482,19 +4482,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F21" t="s">
         <v>597</v>
       </c>
       <c r="G21" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I21" t="s">
         <v>43</v>
@@ -4514,19 +4514,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F22" t="s">
         <v>597</v>
       </c>
       <c r="G22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I22" t="s">
         <v>46</v>
@@ -4546,19 +4546,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F23" t="s">
         <v>597</v>
       </c>
       <c r="G23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I23" t="s">
         <v>49</v>
@@ -4584,7 +4584,7 @@
         <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E24" t="s">
         <v>677</v>
@@ -4593,7 +4593,7 @@
         <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I24" t="s">
         <v>53</v>
@@ -4622,7 +4622,7 @@
         <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E25" t="s">
         <v>677</v>
@@ -4631,7 +4631,7 @@
         <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I25" t="s">
         <v>56</v>
@@ -4654,19 +4654,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F26" t="s">
         <v>598</v>
       </c>
       <c r="G26" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I26" t="s">
         <v>40</v>
@@ -4686,19 +4686,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C27" t="s">
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F27" t="s">
         <v>598</v>
       </c>
       <c r="G27" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I27" t="s">
         <v>43</v>
@@ -4718,19 +4718,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C28" t="s">
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F28" t="s">
         <v>598</v>
       </c>
       <c r="G28" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I28" t="s">
         <v>46</v>
@@ -4750,19 +4750,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="F29" t="s">
         <v>598</v>
       </c>
       <c r="G29" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I29" t="s">
         <v>49</v>
@@ -4782,13 +4782,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C30" t="s">
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E30" t="s">
         <v>677</v>
@@ -4820,13 +4820,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C31" t="s">
         <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E31" t="s">
         <v>677</v>
@@ -4864,7 +4864,7 @@
         <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E32" t="s">
         <v>677</v>
@@ -4902,16 +4902,16 @@
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F33" t="s">
         <v>600</v>
       </c>
       <c r="G33" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H33" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I33" t="s">
         <v>74</v>
@@ -4931,34 +4931,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C34" t="s">
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="F34" t="s">
         <v>600</v>
       </c>
       <c r="G34" t="s">
+        <v>949</v>
+      </c>
+      <c r="H34" t="s">
         <v>950</v>
       </c>
-      <c r="H34" t="s">
-        <v>951</v>
-      </c>
       <c r="I34" t="s">
+        <v>993</v>
+      </c>
+      <c r="K34" t="s">
         <v>994</v>
-      </c>
-      <c r="K34" t="s">
-        <v>995</v>
       </c>
       <c r="L34" t="s">
         <v>73</v>
       </c>
       <c r="M34" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -4972,16 +4972,16 @@
         <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="F35" t="s">
         <v>600</v>
       </c>
       <c r="G35" t="s">
+        <v>951</v>
+      </c>
+      <c r="H35" t="s">
         <v>952</v>
-      </c>
-      <c r="H35" t="s">
-        <v>953</v>
       </c>
       <c r="I35" t="s">
         <v>78</v>
@@ -5001,22 +5001,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C36" t="s">
         <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="F36" t="s">
         <v>600</v>
       </c>
       <c r="G36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H36" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I36" t="s">
         <v>81</v>
@@ -5036,34 +5036,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C37" t="s">
         <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="F37" t="s">
         <v>600</v>
       </c>
       <c r="G37" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H37" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I37" t="s">
+        <v>995</v>
+      </c>
+      <c r="K37" t="s">
         <v>996</v>
-      </c>
-      <c r="K37" t="s">
-        <v>997</v>
       </c>
       <c r="L37" t="s">
         <v>73</v>
       </c>
       <c r="M37" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -5071,22 +5071,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C38" t="s">
         <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="F38" t="s">
         <v>600</v>
       </c>
       <c r="G38" t="s">
+        <v>954</v>
+      </c>
+      <c r="H38" t="s">
         <v>955</v>
-      </c>
-      <c r="H38" t="s">
-        <v>956</v>
       </c>
       <c r="I38" t="s">
         <v>85</v>
@@ -5106,22 +5106,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C39" t="s">
         <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="F39" t="s">
         <v>600</v>
       </c>
       <c r="G39" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H39" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I39" t="s">
         <v>88</v>
@@ -5141,22 +5141,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="F40" t="s">
         <v>600</v>
       </c>
       <c r="G40" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H40" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I40" t="s">
         <v>91</v>
@@ -5176,34 +5176,34 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C41" t="s">
         <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="F41" t="s">
         <v>600</v>
       </c>
       <c r="G41" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H41" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I41" t="s">
+        <v>998</v>
+      </c>
+      <c r="K41" t="s">
         <v>999</v>
-      </c>
-      <c r="K41" t="s">
-        <v>1000</v>
       </c>
       <c r="L41" t="s">
         <v>73</v>
       </c>
       <c r="M41" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -5211,22 +5211,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C42" t="s">
         <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="F42" t="s">
         <v>600</v>
       </c>
       <c r="G42" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="H42" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I42" t="s">
         <v>95</v>
@@ -5246,34 +5246,34 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C43" t="s">
         <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="F43" t="s">
         <v>600</v>
       </c>
       <c r="G43" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="H43" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I43" t="s">
+        <v>1001</v>
+      </c>
+      <c r="K43" t="s">
         <v>1002</v>
-      </c>
-      <c r="K43" t="s">
-        <v>1003</v>
       </c>
       <c r="L43" t="s">
         <v>73</v>
       </c>
       <c r="M43" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -5281,22 +5281,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C44" t="s">
         <v>97</v>
       </c>
       <c r="D44" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="F44" t="s">
         <v>600</v>
       </c>
       <c r="G44" t="s">
+        <v>959</v>
+      </c>
+      <c r="H44" t="s">
         <v>960</v>
-      </c>
-      <c r="H44" t="s">
-        <v>961</v>
       </c>
       <c r="I44" t="s">
         <v>99</v>
@@ -5316,22 +5316,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C45" t="s">
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="F45" t="s">
         <v>600</v>
       </c>
       <c r="G45" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="H45" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I45" t="s">
         <v>102</v>
@@ -5351,19 +5351,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C46" t="s">
         <v>103</v>
       </c>
       <c r="D46" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="F46" t="s">
         <v>600</v>
       </c>
       <c r="G46" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I46" t="s">
         <v>105</v>
@@ -5389,13 +5389,13 @@
         <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F47" t="s">
         <v>600</v>
       </c>
       <c r="G47" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I47" t="s">
         <v>108</v>
@@ -5421,16 +5421,16 @@
         <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F48" t="s">
         <v>601</v>
       </c>
       <c r="G48" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H48" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I48" t="s">
         <v>625</v>
@@ -5450,22 +5450,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C49" t="s">
         <v>113</v>
       </c>
       <c r="D49" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F49" t="s">
         <v>601</v>
       </c>
       <c r="G49" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H49" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I49" t="s">
         <v>626</v>
@@ -5485,22 +5485,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C50" t="s">
         <v>116</v>
       </c>
       <c r="D50" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F50" t="s">
         <v>602</v>
       </c>
       <c r="G50" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H50" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I50" t="s">
         <v>625</v>
@@ -5520,22 +5520,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C51" t="s">
         <v>119</v>
       </c>
       <c r="D51" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F51" t="s">
         <v>602</v>
       </c>
       <c r="G51" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H51" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I51" t="s">
         <v>627</v>
@@ -5561,10 +5561,10 @@
         <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="G52" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="K52" t="s">
         <v>123</v>
@@ -5587,13 +5587,13 @@
         <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F53" t="s">
         <v>603</v>
       </c>
       <c r="G53" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H53">
         <v>2021</v>
@@ -5622,13 +5622,13 @@
         <v>128</v>
       </c>
       <c r="D54" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F54" t="s">
         <v>603</v>
       </c>
       <c r="G54" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H54">
         <v>2021</v>
@@ -5657,13 +5657,13 @@
         <v>131</v>
       </c>
       <c r="D55" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F55" t="s">
         <v>603</v>
       </c>
       <c r="G55" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H55">
         <v>2021</v>
@@ -5692,13 +5692,13 @@
         <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F56" t="s">
         <v>603</v>
       </c>
       <c r="G56" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H56">
         <v>2021</v>
@@ -5727,13 +5727,13 @@
         <v>137</v>
       </c>
       <c r="D57" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F57" t="s">
         <v>603</v>
       </c>
       <c r="G57" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H57">
         <v>2021</v>
@@ -5762,13 +5762,13 @@
         <v>140</v>
       </c>
       <c r="D58" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F58" t="s">
         <v>603</v>
       </c>
       <c r="G58" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H58">
         <v>2021</v>
@@ -5797,13 +5797,13 @@
         <v>143</v>
       </c>
       <c r="D59" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F59" t="s">
         <v>603</v>
       </c>
       <c r="G59" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H59">
         <v>2021</v>
@@ -5832,7 +5832,7 @@
         <v>146</v>
       </c>
       <c r="D60" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F60" t="s">
         <v>603</v>
@@ -5867,7 +5867,7 @@
         <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F61" t="s">
         <v>603</v>
@@ -5902,13 +5902,13 @@
         <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F62" t="s">
         <v>604</v>
       </c>
       <c r="G62" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H62">
         <v>2022</v>
@@ -5937,13 +5937,13 @@
         <v>155</v>
       </c>
       <c r="D63" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F63" t="s">
         <v>604</v>
       </c>
       <c r="G63" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H63">
         <v>2022</v>
@@ -5972,13 +5972,13 @@
         <v>158</v>
       </c>
       <c r="D64" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F64" t="s">
         <v>604</v>
       </c>
       <c r="G64" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H64">
         <v>2022</v>
@@ -6007,13 +6007,13 @@
         <v>161</v>
       </c>
       <c r="D65" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F65" t="s">
         <v>604</v>
       </c>
       <c r="G65" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H65">
         <v>2022</v>
@@ -6042,13 +6042,13 @@
         <v>164</v>
       </c>
       <c r="D66" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F66" t="s">
         <v>604</v>
       </c>
       <c r="G66" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H66">
         <v>2022</v>
@@ -6077,13 +6077,13 @@
         <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F67" t="s">
         <v>604</v>
       </c>
       <c r="G67" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H67">
         <v>2022</v>
@@ -6112,13 +6112,13 @@
         <v>170</v>
       </c>
       <c r="D68" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F68" t="s">
         <v>604</v>
       </c>
       <c r="G68" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H68">
         <v>2022</v>
@@ -6147,7 +6147,7 @@
         <v>173</v>
       </c>
       <c r="D69" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F69" t="s">
         <v>604</v>
@@ -6182,7 +6182,7 @@
         <v>176</v>
       </c>
       <c r="D70" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="F70" t="s">
         <v>604</v>
@@ -6217,13 +6217,13 @@
         <v>179</v>
       </c>
       <c r="D71" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F71" t="s">
         <v>605</v>
       </c>
       <c r="G71" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H71" t="s">
         <v>624</v>
@@ -6252,13 +6252,13 @@
         <v>182</v>
       </c>
       <c r="D72" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F72" t="s">
         <v>605</v>
       </c>
       <c r="G72" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H72" t="s">
         <v>624</v>
@@ -6287,13 +6287,13 @@
         <v>185</v>
       </c>
       <c r="D73" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F73" t="s">
         <v>605</v>
       </c>
       <c r="G73" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H73" t="s">
         <v>624</v>
@@ -6322,13 +6322,13 @@
         <v>188</v>
       </c>
       <c r="D74" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F74" t="s">
         <v>605</v>
       </c>
       <c r="G74" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H74" t="s">
         <v>624</v>
@@ -6357,13 +6357,13 @@
         <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="F75" t="s">
         <v>605</v>
       </c>
       <c r="G75" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H75" t="s">
         <v>624</v>
@@ -6392,13 +6392,13 @@
         <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F76" t="s">
         <v>605</v>
       </c>
       <c r="G76" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H76" t="s">
         <v>624</v>
@@ -6427,13 +6427,13 @@
         <v>197</v>
       </c>
       <c r="D77" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="F77" t="s">
         <v>605</v>
       </c>
       <c r="G77" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H77" t="s">
         <v>624</v>
@@ -6462,7 +6462,7 @@
         <v>200</v>
       </c>
       <c r="D78" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="F78" t="s">
         <v>605</v>
@@ -6497,7 +6497,7 @@
         <v>203</v>
       </c>
       <c r="D79" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="F79" t="s">
         <v>605</v>
@@ -6532,7 +6532,7 @@
         <v>206</v>
       </c>
       <c r="D80" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="K80" t="s">
         <v>207</v>
@@ -6555,7 +6555,7 @@
         <v>208</v>
       </c>
       <c r="D81" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="K81" t="s">
         <v>209</v>
@@ -6578,16 +6578,16 @@
         <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="F82" t="s">
         <v>606</v>
       </c>
       <c r="G82" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H82" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I82" t="s">
         <v>213</v>
@@ -6613,16 +6613,16 @@
         <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="F83" t="s">
         <v>606</v>
       </c>
       <c r="G83" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H83" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I83" t="s">
         <v>216</v>
@@ -6642,34 +6642,34 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C84" t="s">
         <v>217</v>
       </c>
       <c r="D84" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="F84" t="s">
         <v>606</v>
       </c>
       <c r="G84" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H84" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I84" t="s">
+        <v>1004</v>
+      </c>
+      <c r="K84" t="s">
         <v>1005</v>
-      </c>
-      <c r="K84" t="s">
-        <v>1006</v>
       </c>
       <c r="L84" t="s">
         <v>212</v>
       </c>
       <c r="M84" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
@@ -6683,16 +6683,16 @@
         <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="F85" t="s">
         <v>606</v>
       </c>
       <c r="G85" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H85" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I85" t="s">
         <v>220</v>
@@ -6712,34 +6712,34 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C86" t="s">
         <v>221</v>
       </c>
       <c r="D86" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="F86" t="s">
         <v>606</v>
       </c>
       <c r="G86" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H86" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I86" t="s">
+        <v>1007</v>
+      </c>
+      <c r="K86" t="s">
         <v>1008</v>
-      </c>
-      <c r="K86" t="s">
-        <v>1009</v>
       </c>
       <c r="L86" t="s">
         <v>212</v>
       </c>
       <c r="M86" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
@@ -6753,16 +6753,16 @@
         <v>222</v>
       </c>
       <c r="D87" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="F87" t="s">
         <v>606</v>
       </c>
       <c r="G87" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H87" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I87" t="s">
         <v>224</v>
@@ -6782,34 +6782,34 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C88" t="s">
         <v>225</v>
       </c>
       <c r="D88" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F88" t="s">
         <v>606</v>
       </c>
       <c r="G88" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="H88" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I88" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K88" t="s">
         <v>1011</v>
-      </c>
-      <c r="K88" t="s">
-        <v>1012</v>
       </c>
       <c r="L88" t="s">
         <v>212</v>
       </c>
       <c r="M88" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
@@ -6823,16 +6823,16 @@
         <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="F89" t="s">
         <v>606</v>
       </c>
       <c r="G89" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H89" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I89" t="s">
         <v>228</v>
@@ -6852,22 +6852,22 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C90" t="s">
         <v>229</v>
       </c>
       <c r="D90" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="F90" t="s">
         <v>606</v>
       </c>
       <c r="G90" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H90" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I90" t="s">
         <v>231</v>
@@ -6893,7 +6893,7 @@
         <v>232</v>
       </c>
       <c r="D91" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F91" t="s">
         <v>606</v>
@@ -6919,13 +6919,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C92" t="s">
         <v>235</v>
       </c>
       <c r="D92" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="F92" t="s">
         <v>606</v>
@@ -6957,7 +6957,7 @@
         <v>238</v>
       </c>
       <c r="D93" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="K93" t="s">
         <v>239</v>
@@ -6980,16 +6980,16 @@
         <v>242</v>
       </c>
       <c r="D94" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F94" t="s">
         <v>607</v>
       </c>
       <c r="G94" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H94" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I94" t="s">
         <v>652</v>
@@ -7015,16 +7015,16 @@
         <v>246</v>
       </c>
       <c r="D95" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F95" t="s">
         <v>607</v>
       </c>
       <c r="G95" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H95" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I95" t="s">
         <v>653</v>
@@ -7050,16 +7050,16 @@
         <v>249</v>
       </c>
       <c r="D96" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F96" t="s">
         <v>607</v>
       </c>
       <c r="G96" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H96" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="I96" t="s">
         <v>654</v>
@@ -7085,16 +7085,16 @@
         <v>252</v>
       </c>
       <c r="D97" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F97" t="s">
         <v>607</v>
       </c>
       <c r="G97" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H97" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I97" t="s">
         <v>655</v>
@@ -7120,16 +7120,16 @@
         <v>255</v>
       </c>
       <c r="D98" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F98" t="s">
         <v>607</v>
       </c>
       <c r="G98" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H98" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="I98" t="s">
         <v>656</v>
@@ -7155,16 +7155,16 @@
         <v>258</v>
       </c>
       <c r="D99" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="F99" t="s">
         <v>607</v>
       </c>
       <c r="G99" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H99" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I99" t="s">
         <v>657</v>
@@ -7190,16 +7190,16 @@
         <v>261</v>
       </c>
       <c r="D100" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="F100" t="s">
         <v>607</v>
       </c>
       <c r="G100" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H100" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I100" t="s">
         <v>658</v>
@@ -7225,16 +7225,16 @@
         <v>264</v>
       </c>
       <c r="D101" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="F101" t="s">
         <v>608</v>
       </c>
       <c r="G101" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H101" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="I101" t="s">
         <v>267</v>
@@ -7260,16 +7260,16 @@
         <v>268</v>
       </c>
       <c r="D102" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F102" t="s">
         <v>608</v>
       </c>
       <c r="G102" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H102" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="I102" t="s">
         <v>270</v>
@@ -7295,7 +7295,7 @@
         <v>271</v>
       </c>
       <c r="D103" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="F103" t="s">
         <v>609</v>
@@ -7333,7 +7333,7 @@
         <v>275</v>
       </c>
       <c r="D104" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="F104" t="s">
         <v>609</v>
@@ -7342,7 +7342,7 @@
         <v>592</v>
       </c>
       <c r="H104" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="I104" t="s">
         <v>660</v>
@@ -7371,7 +7371,7 @@
         <v>278</v>
       </c>
       <c r="D105" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="F105" t="s">
         <v>609</v>
@@ -7380,7 +7380,7 @@
         <v>592</v>
       </c>
       <c r="H105" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I105" t="s">
         <v>661</v>
@@ -7406,7 +7406,7 @@
         <v>281</v>
       </c>
       <c r="D106" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="F106" t="s">
         <v>609</v>
@@ -7415,7 +7415,7 @@
         <v>592</v>
       </c>
       <c r="H106" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I106" t="s">
         <v>662</v>
@@ -7441,7 +7441,7 @@
         <v>284</v>
       </c>
       <c r="D107" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="F107" t="s">
         <v>609</v>
@@ -7450,7 +7450,7 @@
         <v>592</v>
       </c>
       <c r="H107" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I107" t="s">
         <v>663</v>
@@ -7476,7 +7476,7 @@
         <v>287</v>
       </c>
       <c r="D108" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="F108" t="s">
         <v>609</v>
@@ -7485,7 +7485,7 @@
         <v>592</v>
       </c>
       <c r="H108" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I108" t="s">
         <v>664</v>
@@ -7511,7 +7511,7 @@
         <v>290</v>
       </c>
       <c r="D109" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="F109" t="s">
         <v>609</v>
@@ -7520,7 +7520,7 @@
         <v>592</v>
       </c>
       <c r="H109" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I109" t="s">
         <v>665</v>
@@ -7546,7 +7546,7 @@
         <v>293</v>
       </c>
       <c r="D110" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="F110" t="s">
         <v>609</v>
@@ -7555,7 +7555,7 @@
         <v>592</v>
       </c>
       <c r="H110" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I110" t="s">
         <v>666</v>
@@ -7581,7 +7581,7 @@
         <v>296</v>
       </c>
       <c r="D111" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="F111" t="s">
         <v>609</v>
@@ -7590,7 +7590,7 @@
         <v>592</v>
       </c>
       <c r="H111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I111" t="s">
         <v>667</v>
@@ -7616,7 +7616,7 @@
         <v>299</v>
       </c>
       <c r="D112" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="F112" t="s">
         <v>609</v>
@@ -7625,7 +7625,7 @@
         <v>592</v>
       </c>
       <c r="H112" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I112" t="s">
         <v>668</v>
@@ -7651,7 +7651,7 @@
         <v>302</v>
       </c>
       <c r="D113" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="F113" t="s">
         <v>609</v>
@@ -7660,7 +7660,7 @@
         <v>592</v>
       </c>
       <c r="H113" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I113" t="s">
         <v>669</v>
@@ -7686,7 +7686,7 @@
         <v>305</v>
       </c>
       <c r="D114" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="F114" t="s">
         <v>609</v>
@@ -7695,7 +7695,7 @@
         <v>592</v>
       </c>
       <c r="H114" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I114" t="s">
         <v>670</v>
@@ -7721,7 +7721,7 @@
         <v>308</v>
       </c>
       <c r="D115" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="F115" t="s">
         <v>609</v>
@@ -7730,7 +7730,7 @@
         <v>592</v>
       </c>
       <c r="H115" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I115" t="s">
         <v>671</v>
@@ -7756,7 +7756,7 @@
         <v>311</v>
       </c>
       <c r="D116" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="F116" t="s">
         <v>610</v>
@@ -7791,7 +7791,7 @@
         <v>314</v>
       </c>
       <c r="D117" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="F117" t="s">
         <v>610</v>
@@ -7800,7 +7800,7 @@
         <v>593</v>
       </c>
       <c r="H117" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="I117" t="s">
         <v>660</v>
@@ -7826,7 +7826,7 @@
         <v>317</v>
       </c>
       <c r="D118" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="F118" t="s">
         <v>610</v>
@@ -7835,7 +7835,7 @@
         <v>593</v>
       </c>
       <c r="H118" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I118" t="s">
         <v>661</v>
@@ -7861,7 +7861,7 @@
         <v>320</v>
       </c>
       <c r="D119" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="F119" t="s">
         <v>610</v>
@@ -7870,7 +7870,7 @@
         <v>593</v>
       </c>
       <c r="H119" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I119" t="s">
         <v>662</v>
@@ -7896,7 +7896,7 @@
         <v>323</v>
       </c>
       <c r="D120" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="F120" t="s">
         <v>610</v>
@@ -7905,7 +7905,7 @@
         <v>593</v>
       </c>
       <c r="H120" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I120" t="s">
         <v>663</v>
@@ -7931,7 +7931,7 @@
         <v>326</v>
       </c>
       <c r="D121" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="F121" t="s">
         <v>610</v>
@@ -7940,7 +7940,7 @@
         <v>593</v>
       </c>
       <c r="H121" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I121" t="s">
         <v>664</v>
@@ -7966,7 +7966,7 @@
         <v>329</v>
       </c>
       <c r="D122" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F122" t="s">
         <v>610</v>
@@ -7975,7 +7975,7 @@
         <v>593</v>
       </c>
       <c r="H122" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I122" t="s">
         <v>665</v>
@@ -8001,7 +8001,7 @@
         <v>332</v>
       </c>
       <c r="D123" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="F123" t="s">
         <v>610</v>
@@ -8010,7 +8010,7 @@
         <v>593</v>
       </c>
       <c r="H123" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I123" t="s">
         <v>666</v>
@@ -8036,7 +8036,7 @@
         <v>335</v>
       </c>
       <c r="D124" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="F124" t="s">
         <v>610</v>
@@ -8045,7 +8045,7 @@
         <v>593</v>
       </c>
       <c r="H124" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I124" t="s">
         <v>667</v>
@@ -8071,7 +8071,7 @@
         <v>338</v>
       </c>
       <c r="D125" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="F125" t="s">
         <v>610</v>
@@ -8080,7 +8080,7 @@
         <v>593</v>
       </c>
       <c r="H125" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I125" t="s">
         <v>668</v>
@@ -8106,7 +8106,7 @@
         <v>341</v>
       </c>
       <c r="D126" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="F126" t="s">
         <v>610</v>
@@ -8115,7 +8115,7 @@
         <v>593</v>
       </c>
       <c r="H126" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I126" t="s">
         <v>669</v>
@@ -8141,7 +8141,7 @@
         <v>344</v>
       </c>
       <c r="D127" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F127" t="s">
         <v>610</v>
@@ -8150,7 +8150,7 @@
         <v>593</v>
       </c>
       <c r="H127" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I127" t="s">
         <v>670</v>
@@ -8176,7 +8176,7 @@
         <v>347</v>
       </c>
       <c r="D128" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="F128" t="s">
         <v>610</v>
@@ -8185,7 +8185,7 @@
         <v>593</v>
       </c>
       <c r="H128" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I128" t="s">
         <v>671</v>
@@ -8211,16 +8211,16 @@
         <v>350</v>
       </c>
       <c r="D129" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="F129" t="s">
         <v>611</v>
       </c>
       <c r="G129" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H129" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I129" t="s">
         <v>353</v>
@@ -8249,16 +8249,16 @@
         <v>354</v>
       </c>
       <c r="D130" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="F130" t="s">
         <v>611</v>
       </c>
       <c r="G130" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H130" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I130" t="s">
         <v>356</v>
@@ -8287,16 +8287,16 @@
         <v>357</v>
       </c>
       <c r="D131" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="F131" t="s">
         <v>611</v>
       </c>
       <c r="G131" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H131" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I131" t="s">
         <v>359</v>
@@ -8325,16 +8325,16 @@
         <v>360</v>
       </c>
       <c r="D132" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F132" t="s">
         <v>611</v>
       </c>
       <c r="G132" t="s">
+        <v>892</v>
+      </c>
+      <c r="H132" t="s">
         <v>893</v>
-      </c>
-      <c r="H132" t="s">
-        <v>894</v>
       </c>
       <c r="I132" t="s">
         <v>362</v>
@@ -8363,16 +8363,16 @@
         <v>363</v>
       </c>
       <c r="D133" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="F133" t="s">
         <v>611</v>
       </c>
       <c r="G133" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H133" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="I133" t="s">
         <v>365</v>
@@ -8401,16 +8401,16 @@
         <v>366</v>
       </c>
       <c r="D134" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F134" t="s">
         <v>611</v>
       </c>
       <c r="G134" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H134" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I134" t="s">
         <v>368</v>
@@ -8439,16 +8439,16 @@
         <v>369</v>
       </c>
       <c r="D135" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="F135" t="s">
         <v>611</v>
       </c>
       <c r="G135" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H135" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I135" t="s">
         <v>371</v>
@@ -8477,13 +8477,13 @@
         <v>372</v>
       </c>
       <c r="D136" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F136" t="s">
         <v>611</v>
       </c>
       <c r="G136" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H136" t="s">
         <v>623</v>
@@ -8509,19 +8509,19 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>787</v>
+        <v>1168</v>
       </c>
       <c r="C137" t="s">
         <v>374</v>
       </c>
       <c r="D137" t="s">
-        <v>1061</v>
+        <v>1169</v>
       </c>
       <c r="F137" t="s">
         <v>611</v>
       </c>
       <c r="G137" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H137" t="s">
         <v>623</v>
@@ -8547,13 +8547,13 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C138" t="s">
         <v>376</v>
       </c>
       <c r="D138" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="F138" t="s">
         <v>612</v>
@@ -8576,13 +8576,13 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C139" t="s">
         <v>377</v>
       </c>
       <c r="D139" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="F139" t="s">
         <v>612</v>
@@ -8605,13 +8605,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C140" t="s">
         <v>378</v>
       </c>
       <c r="D140" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="F140" t="s">
         <v>612</v>
@@ -8634,13 +8634,13 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C141" t="s">
         <v>379</v>
       </c>
       <c r="D141" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="F141" t="s">
         <v>612</v>
@@ -8663,22 +8663,22 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C142" t="s">
         <v>380</v>
       </c>
       <c r="D142" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E142" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F142" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G142" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="J142" s="2">
         <v>1</v>
@@ -8698,19 +8698,19 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C143" t="s">
         <v>384</v>
       </c>
       <c r="D143" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E143" t="s">
+        <v>897</v>
+      </c>
+      <c r="F143" t="s">
         <v>898</v>
-      </c>
-      <c r="F143" t="s">
-        <v>899</v>
       </c>
       <c r="K143" t="s">
         <v>385</v>
@@ -8727,19 +8727,19 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C144" t="s">
         <v>387</v>
       </c>
       <c r="D144" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="F144" t="s">
+        <v>898</v>
+      </c>
+      <c r="G144" t="s">
         <v>899</v>
-      </c>
-      <c r="G144" t="s">
-        <v>900</v>
       </c>
       <c r="K144" t="s">
         <v>388</v>
@@ -8756,22 +8756,22 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C145" t="s">
         <v>389</v>
       </c>
       <c r="D145" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E145" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F145" t="s">
+        <v>898</v>
+      </c>
+      <c r="G145" t="s">
         <v>899</v>
-      </c>
-      <c r="G145" t="s">
-        <v>900</v>
       </c>
       <c r="J145" s="2">
         <v>1</v>
@@ -8791,19 +8791,19 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C146" t="s">
         <v>393</v>
       </c>
       <c r="D146" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="F146" t="s">
         <v>613</v>
       </c>
       <c r="G146" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="I146" t="s">
         <v>396</v>
@@ -8823,19 +8823,19 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C147" t="s">
         <v>397</v>
       </c>
       <c r="D147" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="F147" t="s">
         <v>613</v>
       </c>
       <c r="G147" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I147" t="s">
         <v>399</v>
@@ -8855,31 +8855,31 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C148" t="s">
         <v>400</v>
       </c>
       <c r="D148" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F148" t="s">
         <v>613</v>
       </c>
       <c r="G148" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I148" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K148" t="s">
         <v>1015</v>
-      </c>
-      <c r="K148" t="s">
-        <v>1016</v>
       </c>
       <c r="L148" t="s">
         <v>395</v>
       </c>
       <c r="M148" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.3">
@@ -8887,19 +8887,19 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C149" t="s">
         <v>401</v>
       </c>
       <c r="D149" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="F149" t="s">
         <v>613</v>
       </c>
       <c r="G149" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I149" t="s">
         <v>403</v>
@@ -8919,19 +8919,19 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C150" t="s">
         <v>404</v>
       </c>
       <c r="D150" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="F150" t="s">
         <v>613</v>
       </c>
       <c r="G150" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="I150" t="s">
         <v>406</v>
@@ -8951,19 +8951,19 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C151" t="s">
         <v>407</v>
       </c>
       <c r="D151" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="F151" t="s">
         <v>613</v>
       </c>
       <c r="G151" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="I151" t="s">
         <v>409</v>
@@ -8983,13 +8983,13 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C152" t="s">
         <v>410</v>
       </c>
       <c r="D152" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="F152" t="s">
         <v>613</v>
@@ -9015,13 +9015,13 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C153" t="s">
         <v>412</v>
       </c>
       <c r="D153" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="F153" t="s">
         <v>613</v>
@@ -9047,22 +9047,22 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C154" t="s">
         <v>414</v>
       </c>
       <c r="D154" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="F154" t="s">
         <v>614</v>
       </c>
       <c r="G154" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H154" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I154" t="s">
         <v>417</v>
@@ -9082,22 +9082,22 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C155" t="s">
         <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="F155" t="s">
         <v>614</v>
       </c>
       <c r="G155" t="s">
+        <v>904</v>
+      </c>
+      <c r="H155" t="s">
         <v>905</v>
-      </c>
-      <c r="H155" t="s">
-        <v>906</v>
       </c>
       <c r="I155" t="s">
         <v>420</v>
@@ -9117,22 +9117,22 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C156" t="s">
         <v>421</v>
       </c>
       <c r="D156" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="F156" t="s">
         <v>614</v>
       </c>
       <c r="G156" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H156" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I156" t="s">
         <v>423</v>
@@ -9152,22 +9152,22 @@
         <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C157" t="s">
         <v>424</v>
       </c>
       <c r="D157" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="F157" t="s">
         <v>614</v>
       </c>
       <c r="G157" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H157" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I157" t="s">
         <v>426</v>
@@ -9187,22 +9187,22 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C158" t="s">
         <v>427</v>
       </c>
       <c r="D158" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="F158" t="s">
         <v>614</v>
       </c>
       <c r="G158" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H158" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I158" t="s">
         <v>429</v>
@@ -9222,22 +9222,22 @@
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C159" t="s">
         <v>430</v>
       </c>
       <c r="D159" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="F159" t="s">
         <v>614</v>
       </c>
       <c r="G159" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H159" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I159" t="s">
         <v>432</v>
@@ -9257,22 +9257,22 @@
         <v>159</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C160" t="s">
         <v>433</v>
       </c>
       <c r="D160" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="F160" t="s">
         <v>614</v>
       </c>
       <c r="G160" t="s">
+        <v>909</v>
+      </c>
+      <c r="H160" t="s">
         <v>910</v>
-      </c>
-      <c r="H160" t="s">
-        <v>911</v>
       </c>
       <c r="I160" t="s">
         <v>435</v>
@@ -9292,22 +9292,22 @@
         <v>160</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C161" t="s">
         <v>436</v>
       </c>
       <c r="D161" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="F161" t="s">
         <v>614</v>
       </c>
       <c r="G161" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H161" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I161" t="s">
         <v>438</v>
@@ -9327,22 +9327,22 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C162" t="s">
         <v>439</v>
       </c>
       <c r="D162" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="F162" t="s">
         <v>614</v>
       </c>
       <c r="G162" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H162" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I162" t="s">
         <v>441</v>
@@ -9362,13 +9362,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C163" t="s">
         <v>442</v>
       </c>
       <c r="D163" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="F163" t="s">
         <v>614</v>
@@ -9391,13 +9391,13 @@
         <v>163</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C164" t="s">
         <v>444</v>
       </c>
       <c r="D164" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="F164" t="s">
         <v>614</v>
@@ -9420,13 +9420,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C165" t="s">
         <v>446</v>
       </c>
       <c r="D165" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E165" t="s">
         <v>678</v>
@@ -9435,10 +9435,10 @@
         <v>615</v>
       </c>
       <c r="G165" t="s">
+        <v>913</v>
+      </c>
+      <c r="H165" t="s">
         <v>914</v>
-      </c>
-      <c r="H165" t="s">
-        <v>915</v>
       </c>
       <c r="I165" t="s">
         <v>449</v>
@@ -9458,13 +9458,13 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C166" t="s">
         <v>450</v>
       </c>
       <c r="D166" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E166" t="s">
         <v>678</v>
@@ -9473,10 +9473,10 @@
         <v>615</v>
       </c>
       <c r="G166" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H166" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I166" t="s">
         <v>452</v>
@@ -9496,13 +9496,13 @@
         <v>166</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C167" t="s">
         <v>453</v>
       </c>
       <c r="D167" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E167" t="s">
         <v>678</v>
@@ -9511,10 +9511,10 @@
         <v>615</v>
       </c>
       <c r="G167" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H167" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I167" t="s">
         <v>455</v>
@@ -9534,13 +9534,13 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C168" t="s">
         <v>456</v>
       </c>
       <c r="D168" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E168" t="s">
         <v>678</v>
@@ -9549,10 +9549,10 @@
         <v>615</v>
       </c>
       <c r="G168" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H168" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I168" t="s">
         <v>458</v>
@@ -9572,13 +9572,13 @@
         <v>168</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C169" t="s">
         <v>459</v>
       </c>
       <c r="D169" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E169" t="s">
         <v>678</v>
@@ -9587,10 +9587,10 @@
         <v>615</v>
       </c>
       <c r="G169" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H169" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I169" t="s">
         <v>461</v>
@@ -9610,13 +9610,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C170" t="s">
         <v>462</v>
       </c>
       <c r="D170" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E170" t="s">
         <v>678</v>
@@ -9625,7 +9625,7 @@
         <v>615</v>
       </c>
       <c r="G170" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H170" t="s">
         <v>623</v>
@@ -9648,13 +9648,13 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C171" t="s">
         <v>465</v>
       </c>
       <c r="D171" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="E171" t="s">
         <v>678</v>
@@ -9663,7 +9663,7 @@
         <v>615</v>
       </c>
       <c r="G171" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H171" t="s">
         <v>623</v>
@@ -9686,13 +9686,13 @@
         <v>171</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C172" t="s">
         <v>468</v>
       </c>
       <c r="D172" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E172" t="s">
         <v>678</v>
@@ -9701,10 +9701,10 @@
         <v>616</v>
       </c>
       <c r="G172" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H172" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I172" t="s">
         <v>471</v>
@@ -9724,13 +9724,13 @@
         <v>172</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C173" t="s">
         <v>472</v>
       </c>
       <c r="D173" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E173" t="s">
         <v>678</v>
@@ -9739,10 +9739,10 @@
         <v>616</v>
       </c>
       <c r="G173" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H173" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I173" t="s">
         <v>474</v>
@@ -9762,13 +9762,13 @@
         <v>173</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C174" t="s">
         <v>475</v>
       </c>
       <c r="D174" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E174" t="s">
         <v>678</v>
@@ -9777,10 +9777,10 @@
         <v>616</v>
       </c>
       <c r="G174" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H174" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I174" t="s">
         <v>477</v>
@@ -9800,13 +9800,13 @@
         <v>174</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C175" t="s">
         <v>478</v>
       </c>
       <c r="D175" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E175" t="s">
         <v>678</v>
@@ -9815,10 +9815,10 @@
         <v>616</v>
       </c>
       <c r="G175" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H175" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I175" t="s">
         <v>480</v>
@@ -9838,13 +9838,13 @@
         <v>175</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C176" t="s">
         <v>481</v>
       </c>
       <c r="D176" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E176" t="s">
         <v>678</v>
@@ -9853,7 +9853,7 @@
         <v>616</v>
       </c>
       <c r="G176" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H176" t="s">
         <v>623</v>
@@ -9876,13 +9876,13 @@
         <v>176</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C177" t="s">
         <v>483</v>
       </c>
       <c r="D177" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E177" t="s">
         <v>678</v>
@@ -9891,7 +9891,7 @@
         <v>616</v>
       </c>
       <c r="G177" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H177" t="s">
         <v>623</v>
@@ -9914,13 +9914,13 @@
         <v>177</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C178" t="s">
         <v>485</v>
       </c>
       <c r="D178" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E178" t="s">
         <v>678</v>
@@ -9929,10 +9929,10 @@
         <v>617</v>
       </c>
       <c r="G178" t="s">
+        <v>913</v>
+      </c>
+      <c r="H178" t="s">
         <v>914</v>
-      </c>
-      <c r="H178" t="s">
-        <v>915</v>
       </c>
       <c r="I178" t="s">
         <v>449</v>
@@ -9952,13 +9952,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C179" t="s">
         <v>488</v>
       </c>
       <c r="D179" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E179" t="s">
         <v>678</v>
@@ -9967,10 +9967,10 @@
         <v>617</v>
       </c>
       <c r="G179" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H179" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="I179" t="s">
         <v>452</v>
@@ -9990,13 +9990,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C180" t="s">
         <v>490</v>
       </c>
       <c r="D180" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E180" t="s">
         <v>678</v>
@@ -10005,10 +10005,10 @@
         <v>617</v>
       </c>
       <c r="G180" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H180" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I180" t="s">
         <v>455</v>
@@ -10028,13 +10028,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C181" t="s">
         <v>492</v>
       </c>
       <c r="D181" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E181" t="s">
         <v>678</v>
@@ -10043,10 +10043,10 @@
         <v>617</v>
       </c>
       <c r="G181" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H181" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I181" t="s">
         <v>458</v>
@@ -10066,13 +10066,13 @@
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C182" t="s">
         <v>494</v>
       </c>
       <c r="D182" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E182" t="s">
         <v>678</v>
@@ -10081,10 +10081,10 @@
         <v>617</v>
       </c>
       <c r="G182" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H182" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I182" t="s">
         <v>461</v>
@@ -10104,13 +10104,13 @@
         <v>182</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C183" t="s">
         <v>496</v>
       </c>
       <c r="D183" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E183" t="s">
         <v>678</v>
@@ -10119,7 +10119,7 @@
         <v>617</v>
       </c>
       <c r="G183" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H183" t="s">
         <v>623</v>
@@ -10142,13 +10142,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C184" t="s">
         <v>498</v>
       </c>
       <c r="D184" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="E184" t="s">
         <v>678</v>
@@ -10157,7 +10157,7 @@
         <v>617</v>
       </c>
       <c r="G184" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="H184" t="s">
         <v>623</v>
@@ -10180,13 +10180,13 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C185" t="s">
         <v>500</v>
       </c>
       <c r="D185" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E185" t="s">
         <v>678</v>
@@ -10195,10 +10195,10 @@
         <v>618</v>
       </c>
       <c r="G185" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H185" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="I185" t="s">
         <v>503</v>
@@ -10218,13 +10218,13 @@
         <v>185</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C186" t="s">
         <v>504</v>
       </c>
       <c r="D186" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E186" t="s">
         <v>678</v>
@@ -10233,10 +10233,10 @@
         <v>618</v>
       </c>
       <c r="G186" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H186" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I186" t="s">
         <v>506</v>
@@ -10256,13 +10256,13 @@
         <v>186</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C187" t="s">
         <v>507</v>
       </c>
       <c r="D187" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E187" t="s">
         <v>678</v>
@@ -10271,10 +10271,10 @@
         <v>618</v>
       </c>
       <c r="G187" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H187" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I187" t="s">
         <v>477</v>
@@ -10294,13 +10294,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C188" t="s">
         <v>509</v>
       </c>
       <c r="D188" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E188" t="s">
         <v>678</v>
@@ -10309,10 +10309,10 @@
         <v>618</v>
       </c>
       <c r="G188" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H188" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I188" t="s">
         <v>480</v>
@@ -10332,13 +10332,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C189" t="s">
         <v>511</v>
       </c>
       <c r="D189" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E189" t="s">
         <v>678</v>
@@ -10347,7 +10347,7 @@
         <v>618</v>
       </c>
       <c r="G189" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H189" t="s">
         <v>623</v>
@@ -10370,13 +10370,13 @@
         <v>189</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C190" t="s">
         <v>513</v>
       </c>
       <c r="D190" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="E190" t="s">
         <v>678</v>
@@ -10385,7 +10385,7 @@
         <v>618</v>
       </c>
       <c r="G190" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="H190" t="s">
         <v>623</v>
@@ -10408,22 +10408,22 @@
         <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C191" t="s">
         <v>515</v>
       </c>
       <c r="D191" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="E191" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F191" t="s">
         <v>619</v>
       </c>
       <c r="G191" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="I191" t="s">
         <v>518</v>
@@ -10443,22 +10443,22 @@
         <v>191</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C192" t="s">
         <v>519</v>
       </c>
       <c r="D192" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="E192" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F192" t="s">
         <v>619</v>
       </c>
       <c r="G192" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I192" t="s">
         <v>521</v>
@@ -10478,22 +10478,22 @@
         <v>192</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C193" t="s">
         <v>522</v>
       </c>
       <c r="D193" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="E193" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F193" t="s">
         <v>619</v>
       </c>
       <c r="G193" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I193" t="s">
         <v>524</v>
@@ -10513,22 +10513,22 @@
         <v>193</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C194" t="s">
         <v>525</v>
       </c>
       <c r="D194" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E194" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F194" t="s">
         <v>619</v>
       </c>
       <c r="G194" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I194" t="s">
         <v>527</v>
@@ -10548,22 +10548,22 @@
         <v>194</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C195" t="s">
         <v>528</v>
       </c>
       <c r="D195" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="E195" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F195" t="s">
         <v>619</v>
       </c>
       <c r="G195" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="I195" t="s">
         <v>530</v>
@@ -10583,22 +10583,22 @@
         <v>195</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C196" t="s">
         <v>531</v>
       </c>
       <c r="D196" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="E196" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F196" t="s">
         <v>619</v>
       </c>
       <c r="G196" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="I196" t="s">
         <v>533</v>
@@ -10618,22 +10618,22 @@
         <v>196</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C197" t="s">
         <v>534</v>
       </c>
       <c r="D197" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="E197" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F197" t="s">
         <v>619</v>
       </c>
       <c r="G197" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="I197" t="s">
         <v>536</v>
@@ -10653,22 +10653,22 @@
         <v>197</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C198" t="s">
         <v>537</v>
       </c>
       <c r="D198" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="E198" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F198" t="s">
         <v>619</v>
       </c>
       <c r="G198" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I198" t="s">
         <v>539</v>
@@ -10688,22 +10688,22 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C199" t="s">
         <v>540</v>
       </c>
       <c r="D199" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="E199" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F199" t="s">
         <v>619</v>
       </c>
       <c r="G199" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I199" t="s">
         <v>542</v>
@@ -10723,22 +10723,22 @@
         <v>199</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C200" t="s">
         <v>543</v>
       </c>
       <c r="D200" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E200" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F200" t="s">
         <v>619</v>
       </c>
       <c r="G200" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="I200" t="s">
         <v>545</v>
@@ -10758,22 +10758,22 @@
         <v>200</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C201" t="s">
         <v>546</v>
       </c>
       <c r="D201" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="E201" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F201" t="s">
         <v>619</v>
       </c>
       <c r="G201" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I201" t="s">
         <v>548</v>
@@ -10793,22 +10793,22 @@
         <v>201</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C202" t="s">
         <v>549</v>
       </c>
       <c r="D202" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E202" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F202" t="s">
         <v>619</v>
       </c>
       <c r="G202" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I202" t="s">
         <v>551</v>
@@ -10828,22 +10828,22 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C203" t="s">
         <v>552</v>
       </c>
       <c r="D203" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E203" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F203" t="s">
         <v>619</v>
       </c>
       <c r="G203" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I203" t="s">
         <v>554</v>
@@ -10863,13 +10863,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C204" t="s">
         <v>555</v>
       </c>
       <c r="D204" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="K204" t="s">
         <v>556</v>
@@ -10906,7 +10906,7 @@
         <v>559</v>
       </c>
       <c r="D206" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="F206" t="s">
         <v>620</v>
@@ -10935,7 +10935,7 @@
         <v>562</v>
       </c>
       <c r="D207" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="F207" t="s">
         <v>620</v>
@@ -10964,7 +10964,7 @@
         <v>565</v>
       </c>
       <c r="D208" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="F208" t="s">
         <v>620</v>
@@ -11013,7 +11013,7 @@
         <v>570</v>
       </c>
       <c r="D210" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="J210" s="2">
         <v>1</v>
@@ -11076,7 +11076,7 @@
         <v>573</v>
       </c>
       <c r="D213" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="J213" s="2">
         <v>1</v>
@@ -11119,7 +11119,7 @@
         <v>575</v>
       </c>
       <c r="D215" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="K215" t="s">
         <v>575</v>
@@ -11142,7 +11142,7 @@
         <v>576</v>
       </c>
       <c r="D216" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="K216" t="s">
         <v>576</v>
@@ -11222,7 +11222,7 @@
         <v>581</v>
       </c>
       <c r="D220" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="I220" t="s">
         <v>674</v>
@@ -11248,7 +11248,7 @@
         <v>582</v>
       </c>
       <c r="D221" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="J221" s="2">
         <v>1</v>
@@ -11271,7 +11271,7 @@
         <v>583</v>
       </c>
       <c r="D222" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="J222" s="2">
         <v>1</v>
@@ -11317,7 +11317,7 @@
         <v>585</v>
       </c>
       <c r="D224" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="J224" s="2">
         <v>1</v>
@@ -11340,7 +11340,7 @@
         <v>586</v>
       </c>
       <c r="D225" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="J225" s="2">
         <v>1</v>
@@ -11363,7 +11363,7 @@
         <v>587</v>
       </c>
       <c r="D226" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="J226" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Update with correct datatypes
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpoongundranar\Documents\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D50690-37DC-447D-92EF-AE0FDEC01453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF0081-DF4B-4A98-8F5D-2E11B9866702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="1175">
   <si>
     <t>description</t>
   </si>
@@ -3164,9 +3164,6 @@
     <t>Number of paid consultants not applicable</t>
   </si>
   <si>
-    <t>Description of other staff not applicable</t>
-  </si>
-  <si>
     <t>Number of other staff not applicable</t>
   </si>
   <si>
@@ -3558,6 +3555,24 @@
   </si>
   <si>
     <t>names of other revenue sources</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Description of other, not applicable staff</t>
+  </si>
+  <si>
+    <t>Frmajgift</t>
+  </si>
+  <si>
+    <t>CARES</t>
   </si>
 </sst>
 </file>
@@ -4014,8 +4029,8 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4902,7 +4917,10 @@
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>1142</v>
+        <v>1141</v>
+      </c>
+      <c r="E33" t="s">
+        <v>897</v>
       </c>
       <c r="F33" t="s">
         <v>600</v>
@@ -4937,7 +4955,10 @@
         <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>1143</v>
+        <v>1142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>897</v>
       </c>
       <c r="F34" t="s">
         <v>600</v>
@@ -4972,7 +4993,10 @@
         <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>1144</v>
+        <v>1143</v>
+      </c>
+      <c r="E35" t="s">
+        <v>897</v>
       </c>
       <c r="F35" t="s">
         <v>600</v>
@@ -5007,7 +5031,10 @@
         <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>1145</v>
+        <v>1144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>897</v>
       </c>
       <c r="F36" t="s">
         <v>600</v>
@@ -5042,7 +5069,10 @@
         <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>1146</v>
+        <v>1145</v>
+      </c>
+      <c r="E37" t="s">
+        <v>897</v>
       </c>
       <c r="F37" t="s">
         <v>600</v>
@@ -5077,7 +5107,10 @@
         <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>1149</v>
+        <v>1148</v>
+      </c>
+      <c r="E38" t="s">
+        <v>897</v>
       </c>
       <c r="F38" t="s">
         <v>600</v>
@@ -5112,7 +5145,10 @@
         <v>86</v>
       </c>
       <c r="D39" t="s">
-        <v>1150</v>
+        <v>1149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>897</v>
       </c>
       <c r="F39" t="s">
         <v>600</v>
@@ -5147,7 +5183,10 @@
         <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>1151</v>
+        <v>1150</v>
+      </c>
+      <c r="E40" t="s">
+        <v>897</v>
       </c>
       <c r="F40" t="s">
         <v>600</v>
@@ -5182,7 +5221,10 @@
         <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>1147</v>
+        <v>1146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>897</v>
       </c>
       <c r="F41" t="s">
         <v>600</v>
@@ -5217,7 +5259,10 @@
         <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>1152</v>
+        <v>1151</v>
+      </c>
+      <c r="E42" t="s">
+        <v>897</v>
       </c>
       <c r="F42" t="s">
         <v>600</v>
@@ -5252,7 +5297,10 @@
         <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>1148</v>
+        <v>1147</v>
+      </c>
+      <c r="E43" t="s">
+        <v>897</v>
       </c>
       <c r="F43" t="s">
         <v>600</v>
@@ -5287,7 +5335,10 @@
         <v>97</v>
       </c>
       <c r="D44" t="s">
-        <v>1153</v>
+        <v>1152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>897</v>
       </c>
       <c r="F44" t="s">
         <v>600</v>
@@ -5322,7 +5373,10 @@
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>1154</v>
+        <v>1153</v>
+      </c>
+      <c r="E45" t="s">
+        <v>897</v>
       </c>
       <c r="F45" t="s">
         <v>600</v>
@@ -5357,7 +5411,10 @@
         <v>103</v>
       </c>
       <c r="D46" t="s">
-        <v>1155</v>
+        <v>1154</v>
+      </c>
+      <c r="E46" t="s">
+        <v>897</v>
       </c>
       <c r="F46" t="s">
         <v>600</v>
@@ -5391,6 +5448,9 @@
       <c r="D47" t="s">
         <v>1016</v>
       </c>
+      <c r="E47" t="s">
+        <v>1169</v>
+      </c>
       <c r="F47" t="s">
         <v>600</v>
       </c>
@@ -5423,6 +5483,9 @@
       <c r="D48" t="s">
         <v>1017</v>
       </c>
+      <c r="E48" t="s">
+        <v>1170</v>
+      </c>
       <c r="F48" t="s">
         <v>601</v>
       </c>
@@ -5458,6 +5521,9 @@
       <c r="D49" t="s">
         <v>1018</v>
       </c>
+      <c r="E49" t="s">
+        <v>1170</v>
+      </c>
       <c r="F49" t="s">
         <v>601</v>
       </c>
@@ -5493,6 +5559,9 @@
       <c r="D50" t="s">
         <v>1019</v>
       </c>
+      <c r="E50" t="s">
+        <v>897</v>
+      </c>
       <c r="F50" t="s">
         <v>602</v>
       </c>
@@ -5528,6 +5597,9 @@
       <c r="D51" t="s">
         <v>1020</v>
       </c>
+      <c r="E51" t="s">
+        <v>897</v>
+      </c>
       <c r="F51" t="s">
         <v>602</v>
       </c>
@@ -5563,6 +5635,12 @@
       <c r="D52" t="s">
         <v>1021</v>
       </c>
+      <c r="E52" t="s">
+        <v>678</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1171</v>
+      </c>
       <c r="G52" t="s">
         <v>862</v>
       </c>
@@ -5589,6 +5667,9 @@
       <c r="D53" t="s">
         <v>1022</v>
       </c>
+      <c r="E53" t="s">
+        <v>1170</v>
+      </c>
       <c r="F53" t="s">
         <v>603</v>
       </c>
@@ -5624,6 +5705,9 @@
       <c r="D54" t="s">
         <v>1023</v>
       </c>
+      <c r="E54" t="s">
+        <v>1170</v>
+      </c>
       <c r="F54" t="s">
         <v>603</v>
       </c>
@@ -5659,6 +5743,9 @@
       <c r="D55" t="s">
         <v>1024</v>
       </c>
+      <c r="E55" t="s">
+        <v>1170</v>
+      </c>
       <c r="F55" t="s">
         <v>603</v>
       </c>
@@ -5694,6 +5781,9 @@
       <c r="D56" t="s">
         <v>1025</v>
       </c>
+      <c r="E56" t="s">
+        <v>1170</v>
+      </c>
       <c r="F56" t="s">
         <v>603</v>
       </c>
@@ -5729,6 +5819,9 @@
       <c r="D57" t="s">
         <v>1026</v>
       </c>
+      <c r="E57" t="s">
+        <v>1170</v>
+      </c>
       <c r="F57" t="s">
         <v>603</v>
       </c>
@@ -5764,6 +5857,9 @@
       <c r="D58" t="s">
         <v>1027</v>
       </c>
+      <c r="E58" t="s">
+        <v>1170</v>
+      </c>
       <c r="F58" t="s">
         <v>603</v>
       </c>
@@ -5799,6 +5895,9 @@
       <c r="D59" t="s">
         <v>1028</v>
       </c>
+      <c r="E59" t="s">
+        <v>1170</v>
+      </c>
       <c r="F59" t="s">
         <v>603</v>
       </c>
@@ -5834,6 +5933,9 @@
       <c r="D60" t="s">
         <v>1029</v>
       </c>
+      <c r="E60" t="s">
+        <v>1169</v>
+      </c>
       <c r="F60" t="s">
         <v>603</v>
       </c>
@@ -5869,6 +5971,9 @@
       <c r="D61" t="s">
         <v>1030</v>
       </c>
+      <c r="E61" t="s">
+        <v>1170</v>
+      </c>
       <c r="F61" t="s">
         <v>603</v>
       </c>
@@ -5904,6 +6009,9 @@
       <c r="D62" t="s">
         <v>1022</v>
       </c>
+      <c r="E62" t="s">
+        <v>1170</v>
+      </c>
       <c r="F62" t="s">
         <v>604</v>
       </c>
@@ -5939,6 +6047,9 @@
       <c r="D63" t="s">
         <v>1023</v>
       </c>
+      <c r="E63" t="s">
+        <v>1170</v>
+      </c>
       <c r="F63" t="s">
         <v>604</v>
       </c>
@@ -5974,6 +6085,9 @@
       <c r="D64" t="s">
         <v>1024</v>
       </c>
+      <c r="E64" t="s">
+        <v>1170</v>
+      </c>
       <c r="F64" t="s">
         <v>604</v>
       </c>
@@ -6009,6 +6123,9 @@
       <c r="D65" t="s">
         <v>1025</v>
       </c>
+      <c r="E65" t="s">
+        <v>1170</v>
+      </c>
       <c r="F65" t="s">
         <v>604</v>
       </c>
@@ -6044,6 +6161,9 @@
       <c r="D66" t="s">
         <v>1026</v>
       </c>
+      <c r="E66" t="s">
+        <v>1170</v>
+      </c>
       <c r="F66" t="s">
         <v>604</v>
       </c>
@@ -6079,6 +6199,9 @@
       <c r="D67" t="s">
         <v>1027</v>
       </c>
+      <c r="E67" t="s">
+        <v>1170</v>
+      </c>
       <c r="F67" t="s">
         <v>604</v>
       </c>
@@ -6114,6 +6237,9 @@
       <c r="D68" t="s">
         <v>1028</v>
       </c>
+      <c r="E68" t="s">
+        <v>1170</v>
+      </c>
       <c r="F68" t="s">
         <v>604</v>
       </c>
@@ -6149,6 +6275,9 @@
       <c r="D69" t="s">
         <v>1029</v>
       </c>
+      <c r="E69" t="s">
+        <v>1169</v>
+      </c>
       <c r="F69" t="s">
         <v>604</v>
       </c>
@@ -6184,6 +6313,9 @@
       <c r="D70" t="s">
         <v>1030</v>
       </c>
+      <c r="E70" t="s">
+        <v>1170</v>
+      </c>
       <c r="F70" t="s">
         <v>604</v>
       </c>
@@ -6219,6 +6351,9 @@
       <c r="D71" t="s">
         <v>1031</v>
       </c>
+      <c r="E71" t="s">
+        <v>897</v>
+      </c>
       <c r="F71" t="s">
         <v>605</v>
       </c>
@@ -6254,6 +6389,9 @@
       <c r="D72" t="s">
         <v>1032</v>
       </c>
+      <c r="E72" t="s">
+        <v>897</v>
+      </c>
       <c r="F72" t="s">
         <v>605</v>
       </c>
@@ -6289,6 +6427,9 @@
       <c r="D73" t="s">
         <v>1033</v>
       </c>
+      <c r="E73" t="s">
+        <v>897</v>
+      </c>
       <c r="F73" t="s">
         <v>605</v>
       </c>
@@ -6324,6 +6465,9 @@
       <c r="D74" t="s">
         <v>1034</v>
       </c>
+      <c r="E74" t="s">
+        <v>897</v>
+      </c>
       <c r="F74" t="s">
         <v>605</v>
       </c>
@@ -6359,6 +6503,9 @@
       <c r="D75" t="s">
         <v>1035</v>
       </c>
+      <c r="E75" t="s">
+        <v>897</v>
+      </c>
       <c r="F75" t="s">
         <v>605</v>
       </c>
@@ -6394,6 +6541,9 @@
       <c r="D76" t="s">
         <v>1036</v>
       </c>
+      <c r="E76" t="s">
+        <v>897</v>
+      </c>
       <c r="F76" t="s">
         <v>605</v>
       </c>
@@ -6429,6 +6579,9 @@
       <c r="D77" t="s">
         <v>1037</v>
       </c>
+      <c r="E77" t="s">
+        <v>897</v>
+      </c>
       <c r="F77" t="s">
         <v>605</v>
       </c>
@@ -6464,6 +6617,9 @@
       <c r="D78" t="s">
         <v>1038</v>
       </c>
+      <c r="E78" t="s">
+        <v>897</v>
+      </c>
       <c r="F78" t="s">
         <v>605</v>
       </c>
@@ -6497,7 +6653,10 @@
         <v>203</v>
       </c>
       <c r="D79" t="s">
-        <v>1039</v>
+        <v>1172</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1169</v>
       </c>
       <c r="F79" t="s">
         <v>605</v>
@@ -6532,7 +6691,13 @@
         <v>206</v>
       </c>
       <c r="D80" t="s">
-        <v>1140</v>
+        <v>1139</v>
+      </c>
+      <c r="E80" t="s">
+        <v>678</v>
+      </c>
+      <c r="F80" t="s">
+        <v>206</v>
       </c>
       <c r="K80" t="s">
         <v>207</v>
@@ -6555,7 +6720,13 @@
         <v>208</v>
       </c>
       <c r="D81" t="s">
-        <v>1141</v>
+        <v>1140</v>
+      </c>
+      <c r="E81" t="s">
+        <v>678</v>
+      </c>
+      <c r="F81" t="s">
+        <v>208</v>
       </c>
       <c r="K81" t="s">
         <v>209</v>
@@ -6578,7 +6749,10 @@
         <v>210</v>
       </c>
       <c r="D82" t="s">
-        <v>1131</v>
+        <v>1130</v>
+      </c>
+      <c r="E82" t="s">
+        <v>897</v>
       </c>
       <c r="F82" t="s">
         <v>606</v>
@@ -6613,7 +6787,10 @@
         <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>1139</v>
+        <v>1138</v>
+      </c>
+      <c r="E83" t="s">
+        <v>897</v>
       </c>
       <c r="F83" t="s">
         <v>606</v>
@@ -6648,7 +6825,10 @@
         <v>217</v>
       </c>
       <c r="D84" t="s">
-        <v>1135</v>
+        <v>1134</v>
+      </c>
+      <c r="E84" t="s">
+        <v>897</v>
       </c>
       <c r="F84" t="s">
         <v>606</v>
@@ -6683,7 +6863,10 @@
         <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>1132</v>
+        <v>1131</v>
+      </c>
+      <c r="E85" t="s">
+        <v>897</v>
       </c>
       <c r="F85" t="s">
         <v>606</v>
@@ -6718,7 +6901,10 @@
         <v>221</v>
       </c>
       <c r="D86" t="s">
-        <v>1136</v>
+        <v>1135</v>
+      </c>
+      <c r="E86" t="s">
+        <v>897</v>
       </c>
       <c r="F86" t="s">
         <v>606</v>
@@ -6753,7 +6939,10 @@
         <v>222</v>
       </c>
       <c r="D87" t="s">
-        <v>1133</v>
+        <v>1132</v>
+      </c>
+      <c r="E87" t="s">
+        <v>897</v>
       </c>
       <c r="F87" t="s">
         <v>606</v>
@@ -6788,7 +6977,10 @@
         <v>225</v>
       </c>
       <c r="D88" t="s">
-        <v>1137</v>
+        <v>1136</v>
+      </c>
+      <c r="E88" t="s">
+        <v>897</v>
       </c>
       <c r="F88" t="s">
         <v>606</v>
@@ -6823,7 +7015,10 @@
         <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>1134</v>
+        <v>1133</v>
+      </c>
+      <c r="E89" t="s">
+        <v>897</v>
       </c>
       <c r="F89" t="s">
         <v>606</v>
@@ -6858,7 +7053,10 @@
         <v>229</v>
       </c>
       <c r="D90" t="s">
-        <v>1138</v>
+        <v>1137</v>
+      </c>
+      <c r="E90" t="s">
+        <v>897</v>
       </c>
       <c r="F90" t="s">
         <v>606</v>
@@ -6893,7 +7091,10 @@
         <v>232</v>
       </c>
       <c r="D91" t="s">
-        <v>1040</v>
+        <v>1039</v>
+      </c>
+      <c r="E91" t="s">
+        <v>897</v>
       </c>
       <c r="F91" t="s">
         <v>606</v>
@@ -6925,7 +7126,10 @@
         <v>235</v>
       </c>
       <c r="D92" t="s">
-        <v>1041</v>
+        <v>1040</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1169</v>
       </c>
       <c r="F92" t="s">
         <v>606</v>
@@ -6957,7 +7161,13 @@
         <v>238</v>
       </c>
       <c r="D93" t="s">
-        <v>1046</v>
+        <v>1045</v>
+      </c>
+      <c r="E93" t="s">
+        <v>896</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1173</v>
       </c>
       <c r="K93" t="s">
         <v>239</v>
@@ -6980,7 +7190,10 @@
         <v>242</v>
       </c>
       <c r="D94" t="s">
-        <v>1042</v>
+        <v>1041</v>
+      </c>
+      <c r="E94" t="s">
+        <v>678</v>
       </c>
       <c r="F94" t="s">
         <v>607</v>
@@ -7015,7 +7228,10 @@
         <v>246</v>
       </c>
       <c r="D95" t="s">
-        <v>1043</v>
+        <v>1042</v>
+      </c>
+      <c r="E95" t="s">
+        <v>678</v>
       </c>
       <c r="F95" t="s">
         <v>607</v>
@@ -7050,7 +7266,10 @@
         <v>249</v>
       </c>
       <c r="D96" t="s">
-        <v>1044</v>
+        <v>1043</v>
+      </c>
+      <c r="E96" t="s">
+        <v>678</v>
       </c>
       <c r="F96" t="s">
         <v>607</v>
@@ -7085,7 +7304,10 @@
         <v>252</v>
       </c>
       <c r="D97" t="s">
-        <v>1045</v>
+        <v>1044</v>
+      </c>
+      <c r="E97" t="s">
+        <v>678</v>
       </c>
       <c r="F97" t="s">
         <v>607</v>
@@ -7120,7 +7342,10 @@
         <v>255</v>
       </c>
       <c r="D98" t="s">
-        <v>1047</v>
+        <v>1046</v>
+      </c>
+      <c r="E98" t="s">
+        <v>678</v>
       </c>
       <c r="F98" t="s">
         <v>607</v>
@@ -7155,7 +7380,10 @@
         <v>258</v>
       </c>
       <c r="D99" t="s">
-        <v>1048</v>
+        <v>1047</v>
+      </c>
+      <c r="E99" t="s">
+        <v>678</v>
       </c>
       <c r="F99" t="s">
         <v>607</v>
@@ -7190,7 +7418,10 @@
         <v>261</v>
       </c>
       <c r="D100" t="s">
-        <v>1049</v>
+        <v>1048</v>
+      </c>
+      <c r="E100" t="s">
+        <v>678</v>
       </c>
       <c r="F100" t="s">
         <v>607</v>
@@ -7225,7 +7456,10 @@
         <v>264</v>
       </c>
       <c r="D101" t="s">
-        <v>1050</v>
+        <v>1049</v>
+      </c>
+      <c r="E101" t="s">
+        <v>1170</v>
       </c>
       <c r="F101" t="s">
         <v>608</v>
@@ -7260,7 +7494,10 @@
         <v>268</v>
       </c>
       <c r="D102" t="s">
-        <v>1051</v>
+        <v>1050</v>
+      </c>
+      <c r="E102" t="s">
+        <v>1170</v>
       </c>
       <c r="F102" t="s">
         <v>608</v>
@@ -7295,7 +7532,10 @@
         <v>271</v>
       </c>
       <c r="D103" t="s">
-        <v>1105</v>
+        <v>1104</v>
+      </c>
+      <c r="E103" t="s">
+        <v>897</v>
       </c>
       <c r="F103" t="s">
         <v>609</v>
@@ -7333,7 +7573,10 @@
         <v>275</v>
       </c>
       <c r="D104" t="s">
-        <v>1106</v>
+        <v>1105</v>
+      </c>
+      <c r="E104" t="s">
+        <v>897</v>
       </c>
       <c r="F104" t="s">
         <v>609</v>
@@ -7371,7 +7614,10 @@
         <v>278</v>
       </c>
       <c r="D105" t="s">
-        <v>1107</v>
+        <v>1106</v>
+      </c>
+      <c r="E105" t="s">
+        <v>897</v>
       </c>
       <c r="F105" t="s">
         <v>609</v>
@@ -7406,7 +7652,10 @@
         <v>281</v>
       </c>
       <c r="D106" t="s">
-        <v>1108</v>
+        <v>1107</v>
+      </c>
+      <c r="E106" t="s">
+        <v>897</v>
       </c>
       <c r="F106" t="s">
         <v>609</v>
@@ -7441,7 +7690,10 @@
         <v>284</v>
       </c>
       <c r="D107" t="s">
-        <v>1109</v>
+        <v>1108</v>
+      </c>
+      <c r="E107" t="s">
+        <v>897</v>
       </c>
       <c r="F107" t="s">
         <v>609</v>
@@ -7476,7 +7728,10 @@
         <v>287</v>
       </c>
       <c r="D108" t="s">
-        <v>1110</v>
+        <v>1109</v>
+      </c>
+      <c r="E108" t="s">
+        <v>897</v>
       </c>
       <c r="F108" t="s">
         <v>609</v>
@@ -7511,7 +7766,10 @@
         <v>290</v>
       </c>
       <c r="D109" t="s">
-        <v>1111</v>
+        <v>1110</v>
+      </c>
+      <c r="E109" t="s">
+        <v>897</v>
       </c>
       <c r="F109" t="s">
         <v>609</v>
@@ -7546,7 +7804,10 @@
         <v>293</v>
       </c>
       <c r="D110" t="s">
-        <v>1112</v>
+        <v>1111</v>
+      </c>
+      <c r="E110" t="s">
+        <v>897</v>
       </c>
       <c r="F110" t="s">
         <v>609</v>
@@ -7581,7 +7842,10 @@
         <v>296</v>
       </c>
       <c r="D111" t="s">
-        <v>1113</v>
+        <v>1112</v>
+      </c>
+      <c r="E111" t="s">
+        <v>897</v>
       </c>
       <c r="F111" t="s">
         <v>609</v>
@@ -7616,7 +7880,10 @@
         <v>299</v>
       </c>
       <c r="D112" t="s">
-        <v>1114</v>
+        <v>1113</v>
+      </c>
+      <c r="E112" t="s">
+        <v>897</v>
       </c>
       <c r="F112" t="s">
         <v>609</v>
@@ -7651,7 +7918,10 @@
         <v>302</v>
       </c>
       <c r="D113" t="s">
-        <v>1115</v>
+        <v>1114</v>
+      </c>
+      <c r="E113" t="s">
+        <v>897</v>
       </c>
       <c r="F113" t="s">
         <v>609</v>
@@ -7686,7 +7956,10 @@
         <v>305</v>
       </c>
       <c r="D114" t="s">
-        <v>1116</v>
+        <v>1115</v>
+      </c>
+      <c r="E114" t="s">
+        <v>897</v>
       </c>
       <c r="F114" t="s">
         <v>609</v>
@@ -7721,7 +7994,10 @@
         <v>308</v>
       </c>
       <c r="D115" t="s">
-        <v>1117</v>
+        <v>1116</v>
+      </c>
+      <c r="E115" t="s">
+        <v>897</v>
       </c>
       <c r="F115" t="s">
         <v>609</v>
@@ -7756,7 +8032,10 @@
         <v>311</v>
       </c>
       <c r="D116" t="s">
-        <v>1118</v>
+        <v>1117</v>
+      </c>
+      <c r="E116" t="s">
+        <v>897</v>
       </c>
       <c r="F116" t="s">
         <v>610</v>
@@ -7791,7 +8070,10 @@
         <v>314</v>
       </c>
       <c r="D117" t="s">
-        <v>1119</v>
+        <v>1118</v>
+      </c>
+      <c r="E117" t="s">
+        <v>897</v>
       </c>
       <c r="F117" t="s">
         <v>610</v>
@@ -7826,7 +8108,10 @@
         <v>317</v>
       </c>
       <c r="D118" t="s">
-        <v>1120</v>
+        <v>1119</v>
+      </c>
+      <c r="E118" t="s">
+        <v>897</v>
       </c>
       <c r="F118" t="s">
         <v>610</v>
@@ -7861,7 +8146,10 @@
         <v>320</v>
       </c>
       <c r="D119" t="s">
-        <v>1121</v>
+        <v>1120</v>
+      </c>
+      <c r="E119" t="s">
+        <v>897</v>
       </c>
       <c r="F119" t="s">
         <v>610</v>
@@ -7896,7 +8184,10 @@
         <v>323</v>
       </c>
       <c r="D120" t="s">
-        <v>1122</v>
+        <v>1121</v>
+      </c>
+      <c r="E120" t="s">
+        <v>897</v>
       </c>
       <c r="F120" t="s">
         <v>610</v>
@@ -7931,7 +8222,10 @@
         <v>326</v>
       </c>
       <c r="D121" t="s">
-        <v>1123</v>
+        <v>1122</v>
+      </c>
+      <c r="E121" t="s">
+        <v>897</v>
       </c>
       <c r="F121" t="s">
         <v>610</v>
@@ -7966,7 +8260,10 @@
         <v>329</v>
       </c>
       <c r="D122" t="s">
-        <v>1124</v>
+        <v>1123</v>
+      </c>
+      <c r="E122" t="s">
+        <v>897</v>
       </c>
       <c r="F122" t="s">
         <v>610</v>
@@ -8001,7 +8298,10 @@
         <v>332</v>
       </c>
       <c r="D123" t="s">
-        <v>1125</v>
+        <v>1124</v>
+      </c>
+      <c r="E123" t="s">
+        <v>897</v>
       </c>
       <c r="F123" t="s">
         <v>610</v>
@@ -8036,7 +8336,10 @@
         <v>335</v>
       </c>
       <c r="D124" t="s">
-        <v>1126</v>
+        <v>1125</v>
+      </c>
+      <c r="E124" t="s">
+        <v>897</v>
       </c>
       <c r="F124" t="s">
         <v>610</v>
@@ -8071,7 +8374,10 @@
         <v>338</v>
       </c>
       <c r="D125" t="s">
-        <v>1127</v>
+        <v>1126</v>
+      </c>
+      <c r="E125" t="s">
+        <v>897</v>
       </c>
       <c r="F125" t="s">
         <v>610</v>
@@ -8106,7 +8412,10 @@
         <v>341</v>
       </c>
       <c r="D126" t="s">
-        <v>1128</v>
+        <v>1127</v>
+      </c>
+      <c r="E126" t="s">
+        <v>897</v>
       </c>
       <c r="F126" t="s">
         <v>610</v>
@@ -8141,7 +8450,10 @@
         <v>344</v>
       </c>
       <c r="D127" t="s">
-        <v>1129</v>
+        <v>1128</v>
+      </c>
+      <c r="E127" t="s">
+        <v>897</v>
       </c>
       <c r="F127" t="s">
         <v>610</v>
@@ -8176,7 +8488,10 @@
         <v>347</v>
       </c>
       <c r="D128" t="s">
-        <v>1130</v>
+        <v>1129</v>
+      </c>
+      <c r="E128" t="s">
+        <v>897</v>
       </c>
       <c r="F128" t="s">
         <v>610</v>
@@ -8211,7 +8526,10 @@
         <v>350</v>
       </c>
       <c r="D129" t="s">
-        <v>1052</v>
+        <v>1051</v>
+      </c>
+      <c r="E129" t="s">
+        <v>896</v>
       </c>
       <c r="F129" t="s">
         <v>611</v>
@@ -8249,7 +8567,10 @@
         <v>354</v>
       </c>
       <c r="D130" t="s">
-        <v>1053</v>
+        <v>1052</v>
+      </c>
+      <c r="E130" t="s">
+        <v>896</v>
       </c>
       <c r="F130" t="s">
         <v>611</v>
@@ -8287,7 +8608,10 @@
         <v>357</v>
       </c>
       <c r="D131" t="s">
-        <v>1054</v>
+        <v>1053</v>
+      </c>
+      <c r="E131" t="s">
+        <v>896</v>
       </c>
       <c r="F131" t="s">
         <v>611</v>
@@ -8325,7 +8649,10 @@
         <v>360</v>
       </c>
       <c r="D132" t="s">
-        <v>1055</v>
+        <v>1054</v>
+      </c>
+      <c r="E132" t="s">
+        <v>896</v>
       </c>
       <c r="F132" t="s">
         <v>611</v>
@@ -8363,7 +8690,10 @@
         <v>363</v>
       </c>
       <c r="D133" t="s">
-        <v>1056</v>
+        <v>1055</v>
+      </c>
+      <c r="E133" t="s">
+        <v>896</v>
       </c>
       <c r="F133" t="s">
         <v>611</v>
@@ -8401,7 +8731,10 @@
         <v>366</v>
       </c>
       <c r="D134" t="s">
-        <v>1057</v>
+        <v>1056</v>
+      </c>
+      <c r="E134" t="s">
+        <v>896</v>
       </c>
       <c r="F134" t="s">
         <v>611</v>
@@ -8439,7 +8772,10 @@
         <v>369</v>
       </c>
       <c r="D135" t="s">
-        <v>1058</v>
+        <v>1057</v>
+      </c>
+      <c r="E135" t="s">
+        <v>896</v>
       </c>
       <c r="F135" t="s">
         <v>611</v>
@@ -8477,7 +8813,10 @@
         <v>372</v>
       </c>
       <c r="D136" t="s">
-        <v>1059</v>
+        <v>1058</v>
+      </c>
+      <c r="E136" t="s">
+        <v>896</v>
       </c>
       <c r="F136" t="s">
         <v>611</v>
@@ -8509,12 +8848,15 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C137" t="s">
         <v>374</v>
       </c>
       <c r="D137" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E137" t="s">
         <v>1169</v>
       </c>
       <c r="F137" t="s">
@@ -8553,7 +8895,7 @@
         <v>376</v>
       </c>
       <c r="D138" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F138" t="s">
         <v>612</v>
@@ -8582,7 +8924,7 @@
         <v>377</v>
       </c>
       <c r="D139" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F139" t="s">
         <v>612</v>
@@ -8611,7 +8953,7 @@
         <v>378</v>
       </c>
       <c r="D140" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="F140" t="s">
         <v>612</v>
@@ -8640,7 +8982,7 @@
         <v>379</v>
       </c>
       <c r="D141" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F141" t="s">
         <v>612</v>
@@ -8669,7 +9011,7 @@
         <v>380</v>
       </c>
       <c r="D142" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E142" t="s">
         <v>896</v>
@@ -8704,7 +9046,7 @@
         <v>384</v>
       </c>
       <c r="D143" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E143" t="s">
         <v>897</v>
@@ -8733,10 +9075,13 @@
         <v>387</v>
       </c>
       <c r="D144" t="s">
-        <v>1066</v>
+        <v>1065</v>
+      </c>
+      <c r="E144" t="s">
+        <v>897</v>
       </c>
       <c r="F144" t="s">
-        <v>898</v>
+        <v>1174</v>
       </c>
       <c r="G144" t="s">
         <v>899</v>
@@ -8762,13 +9107,13 @@
         <v>389</v>
       </c>
       <c r="D145" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E145" t="s">
         <v>896</v>
       </c>
       <c r="F145" t="s">
-        <v>898</v>
+        <v>1174</v>
       </c>
       <c r="G145" t="s">
         <v>899</v>
@@ -8797,7 +9142,10 @@
         <v>393</v>
       </c>
       <c r="D146" t="s">
-        <v>1068</v>
+        <v>1067</v>
+      </c>
+      <c r="E146" t="s">
+        <v>897</v>
       </c>
       <c r="F146" t="s">
         <v>613</v>
@@ -8829,7 +9177,10 @@
         <v>397</v>
       </c>
       <c r="D147" t="s">
-        <v>1069</v>
+        <v>1068</v>
+      </c>
+      <c r="E147" t="s">
+        <v>897</v>
       </c>
       <c r="F147" t="s">
         <v>613</v>
@@ -8861,7 +9212,10 @@
         <v>400</v>
       </c>
       <c r="D148" t="s">
-        <v>1070</v>
+        <v>1069</v>
+      </c>
+      <c r="E148" t="s">
+        <v>897</v>
       </c>
       <c r="F148" t="s">
         <v>613</v>
@@ -8893,7 +9247,10 @@
         <v>401</v>
       </c>
       <c r="D149" t="s">
-        <v>1071</v>
+        <v>1070</v>
+      </c>
+      <c r="E149" t="s">
+        <v>897</v>
       </c>
       <c r="F149" t="s">
         <v>613</v>
@@ -8925,7 +9282,10 @@
         <v>404</v>
       </c>
       <c r="D150" t="s">
-        <v>1072</v>
+        <v>1071</v>
+      </c>
+      <c r="E150" t="s">
+        <v>897</v>
       </c>
       <c r="F150" t="s">
         <v>613</v>
@@ -8951,13 +9311,16 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C151" t="s">
         <v>407</v>
       </c>
       <c r="D151" t="s">
-        <v>1073</v>
+        <v>1072</v>
+      </c>
+      <c r="E151" t="s">
+        <v>897</v>
       </c>
       <c r="F151" t="s">
         <v>613</v>
@@ -8989,7 +9352,10 @@
         <v>410</v>
       </c>
       <c r="D152" t="s">
-        <v>1074</v>
+        <v>1073</v>
+      </c>
+      <c r="E152" t="s">
+        <v>897</v>
       </c>
       <c r="F152" t="s">
         <v>613</v>
@@ -9021,7 +9387,10 @@
         <v>412</v>
       </c>
       <c r="D153" t="s">
-        <v>1075</v>
+        <v>1074</v>
+      </c>
+      <c r="E153" t="s">
+        <v>1169</v>
       </c>
       <c r="F153" t="s">
         <v>613</v>
@@ -9053,7 +9422,10 @@
         <v>414</v>
       </c>
       <c r="D154" t="s">
-        <v>1076</v>
+        <v>1075</v>
+      </c>
+      <c r="E154" t="s">
+        <v>897</v>
       </c>
       <c r="F154" t="s">
         <v>614</v>
@@ -9088,7 +9460,10 @@
         <v>418</v>
       </c>
       <c r="D155" t="s">
-        <v>1077</v>
+        <v>1076</v>
+      </c>
+      <c r="E155" t="s">
+        <v>897</v>
       </c>
       <c r="F155" t="s">
         <v>614</v>
@@ -9123,7 +9498,10 @@
         <v>421</v>
       </c>
       <c r="D156" t="s">
-        <v>1078</v>
+        <v>1077</v>
+      </c>
+      <c r="E156" t="s">
+        <v>897</v>
       </c>
       <c r="F156" t="s">
         <v>614</v>
@@ -9158,7 +9536,10 @@
         <v>424</v>
       </c>
       <c r="D157" t="s">
-        <v>1079</v>
+        <v>1078</v>
+      </c>
+      <c r="E157" t="s">
+        <v>897</v>
       </c>
       <c r="F157" t="s">
         <v>614</v>
@@ -9193,7 +9574,10 @@
         <v>427</v>
       </c>
       <c r="D158" t="s">
-        <v>1080</v>
+        <v>1079</v>
+      </c>
+      <c r="E158" t="s">
+        <v>897</v>
       </c>
       <c r="F158" t="s">
         <v>614</v>
@@ -9228,7 +9612,10 @@
         <v>430</v>
       </c>
       <c r="D159" t="s">
-        <v>1081</v>
+        <v>1080</v>
+      </c>
+      <c r="E159" t="s">
+        <v>897</v>
       </c>
       <c r="F159" t="s">
         <v>614</v>
@@ -9263,7 +9650,10 @@
         <v>433</v>
       </c>
       <c r="D160" t="s">
-        <v>1082</v>
+        <v>1081</v>
+      </c>
+      <c r="E160" t="s">
+        <v>897</v>
       </c>
       <c r="F160" t="s">
         <v>614</v>
@@ -9298,7 +9688,10 @@
         <v>436</v>
       </c>
       <c r="D161" t="s">
-        <v>1083</v>
+        <v>1082</v>
+      </c>
+      <c r="E161" t="s">
+        <v>897</v>
       </c>
       <c r="F161" t="s">
         <v>614</v>
@@ -9333,7 +9726,10 @@
         <v>439</v>
       </c>
       <c r="D162" t="s">
-        <v>1084</v>
+        <v>1083</v>
+      </c>
+      <c r="E162" t="s">
+        <v>897</v>
       </c>
       <c r="F162" t="s">
         <v>614</v>
@@ -9368,7 +9764,10 @@
         <v>442</v>
       </c>
       <c r="D163" t="s">
-        <v>1085</v>
+        <v>1084</v>
+      </c>
+      <c r="E163" t="s">
+        <v>897</v>
       </c>
       <c r="F163" t="s">
         <v>614</v>
@@ -9397,7 +9796,10 @@
         <v>444</v>
       </c>
       <c r="D164" t="s">
-        <v>1086</v>
+        <v>1085</v>
+      </c>
+      <c r="E164" t="s">
+        <v>1169</v>
       </c>
       <c r="F164" t="s">
         <v>614</v>
@@ -9426,10 +9828,10 @@
         <v>446</v>
       </c>
       <c r="D165" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E165" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F165" t="s">
         <v>615</v>
@@ -9464,10 +9866,10 @@
         <v>450</v>
       </c>
       <c r="D166" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E166" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F166" t="s">
         <v>615</v>
@@ -9502,10 +9904,10 @@
         <v>453</v>
       </c>
       <c r="D167" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E167" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F167" t="s">
         <v>615</v>
@@ -9540,10 +9942,10 @@
         <v>456</v>
       </c>
       <c r="D168" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E168" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F168" t="s">
         <v>615</v>
@@ -9578,10 +9980,10 @@
         <v>459</v>
       </c>
       <c r="D169" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E169" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F169" t="s">
         <v>615</v>
@@ -9616,10 +10018,10 @@
         <v>462</v>
       </c>
       <c r="D170" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E170" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F170" t="s">
         <v>615</v>
@@ -9654,10 +10056,10 @@
         <v>465</v>
       </c>
       <c r="D171" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E171" t="s">
-        <v>678</v>
+        <v>1169</v>
       </c>
       <c r="F171" t="s">
         <v>615</v>
@@ -9692,10 +10094,10 @@
         <v>468</v>
       </c>
       <c r="D172" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E172" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F172" t="s">
         <v>616</v>
@@ -9730,10 +10132,10 @@
         <v>472</v>
       </c>
       <c r="D173" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E173" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F173" t="s">
         <v>616</v>
@@ -9768,10 +10170,10 @@
         <v>475</v>
       </c>
       <c r="D174" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E174" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F174" t="s">
         <v>616</v>
@@ -9806,10 +10208,10 @@
         <v>478</v>
       </c>
       <c r="D175" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E175" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F175" t="s">
         <v>616</v>
@@ -9844,10 +10246,10 @@
         <v>481</v>
       </c>
       <c r="D176" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E176" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F176" t="s">
         <v>616</v>
@@ -9882,10 +10284,10 @@
         <v>483</v>
       </c>
       <c r="D177" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E177" t="s">
-        <v>678</v>
+        <v>1169</v>
       </c>
       <c r="F177" t="s">
         <v>616</v>
@@ -9920,10 +10322,10 @@
         <v>485</v>
       </c>
       <c r="D178" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E178" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F178" t="s">
         <v>617</v>
@@ -9958,10 +10360,10 @@
         <v>488</v>
       </c>
       <c r="D179" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E179" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F179" t="s">
         <v>617</v>
@@ -9996,10 +10398,10 @@
         <v>490</v>
       </c>
       <c r="D180" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E180" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F180" t="s">
         <v>617</v>
@@ -10034,10 +10436,10 @@
         <v>492</v>
       </c>
       <c r="D181" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E181" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F181" t="s">
         <v>617</v>
@@ -10072,10 +10474,10 @@
         <v>494</v>
       </c>
       <c r="D182" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E182" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F182" t="s">
         <v>617</v>
@@ -10110,10 +10512,10 @@
         <v>496</v>
       </c>
       <c r="D183" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E183" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F183" t="s">
         <v>617</v>
@@ -10148,10 +10550,10 @@
         <v>498</v>
       </c>
       <c r="D184" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E184" t="s">
-        <v>678</v>
+        <v>1169</v>
       </c>
       <c r="F184" t="s">
         <v>617</v>
@@ -10186,10 +10588,10 @@
         <v>500</v>
       </c>
       <c r="D185" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E185" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F185" t="s">
         <v>618</v>
@@ -10224,10 +10626,10 @@
         <v>504</v>
       </c>
       <c r="D186" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E186" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F186" t="s">
         <v>618</v>
@@ -10262,10 +10664,10 @@
         <v>507</v>
       </c>
       <c r="D187" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E187" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F187" t="s">
         <v>618</v>
@@ -10300,10 +10702,10 @@
         <v>509</v>
       </c>
       <c r="D188" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E188" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F188" t="s">
         <v>618</v>
@@ -10338,10 +10740,10 @@
         <v>511</v>
       </c>
       <c r="D189" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E189" t="s">
-        <v>678</v>
+        <v>897</v>
       </c>
       <c r="F189" t="s">
         <v>618</v>
@@ -10376,10 +10778,10 @@
         <v>513</v>
       </c>
       <c r="D190" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E190" t="s">
-        <v>678</v>
+        <v>1169</v>
       </c>
       <c r="F190" t="s">
         <v>618</v>
@@ -10414,10 +10816,10 @@
         <v>515</v>
       </c>
       <c r="D191" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E191" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F191" t="s">
         <v>619</v>
@@ -10449,10 +10851,10 @@
         <v>519</v>
       </c>
       <c r="D192" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E192" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F192" t="s">
         <v>619</v>
@@ -10484,10 +10886,10 @@
         <v>522</v>
       </c>
       <c r="D193" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E193" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F193" t="s">
         <v>619</v>
@@ -10519,10 +10921,10 @@
         <v>525</v>
       </c>
       <c r="D194" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E194" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F194" t="s">
         <v>619</v>
@@ -10554,10 +10956,10 @@
         <v>528</v>
       </c>
       <c r="D195" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E195" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F195" t="s">
         <v>619</v>
@@ -10589,10 +10991,10 @@
         <v>531</v>
       </c>
       <c r="D196" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E196" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F196" t="s">
         <v>619</v>
@@ -10624,10 +11026,10 @@
         <v>534</v>
       </c>
       <c r="D197" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E197" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F197" t="s">
         <v>619</v>
@@ -10659,10 +11061,10 @@
         <v>537</v>
       </c>
       <c r="D198" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E198" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F198" t="s">
         <v>619</v>
@@ -10694,10 +11096,10 @@
         <v>540</v>
       </c>
       <c r="D199" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E199" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F199" t="s">
         <v>619</v>
@@ -10729,10 +11131,10 @@
         <v>543</v>
       </c>
       <c r="D200" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E200" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F200" t="s">
         <v>619</v>
@@ -10764,10 +11166,10 @@
         <v>546</v>
       </c>
       <c r="D201" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E201" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F201" t="s">
         <v>619</v>
@@ -10799,10 +11201,10 @@
         <v>549</v>
       </c>
       <c r="D202" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E202" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F202" t="s">
         <v>619</v>
@@ -10834,10 +11236,10 @@
         <v>552</v>
       </c>
       <c r="D203" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E203" t="s">
-        <v>896</v>
+        <v>678</v>
       </c>
       <c r="F203" t="s">
         <v>619</v>
@@ -10869,7 +11271,13 @@
         <v>555</v>
       </c>
       <c r="D204" t="s">
-        <v>1104</v>
+        <v>1103</v>
+      </c>
+      <c r="E204" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F204" t="s">
+        <v>847</v>
       </c>
       <c r="K204" t="s">
         <v>556</v>
@@ -10906,7 +11314,7 @@
         <v>559</v>
       </c>
       <c r="D206" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F206" t="s">
         <v>620</v>
@@ -10935,7 +11343,7 @@
         <v>562</v>
       </c>
       <c r="D207" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F207" t="s">
         <v>620</v>
@@ -10964,7 +11372,7 @@
         <v>565</v>
       </c>
       <c r="D208" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F208" t="s">
         <v>620</v>
@@ -11013,7 +11421,7 @@
         <v>570</v>
       </c>
       <c r="D210" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="J210" s="2">
         <v>1</v>
@@ -11076,7 +11484,7 @@
         <v>573</v>
       </c>
       <c r="D213" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="J213" s="2">
         <v>1</v>
@@ -11119,7 +11527,7 @@
         <v>575</v>
       </c>
       <c r="D215" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="K215" t="s">
         <v>575</v>
@@ -11142,7 +11550,7 @@
         <v>576</v>
       </c>
       <c r="D216" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="K216" t="s">
         <v>576</v>
@@ -11222,7 +11630,7 @@
         <v>581</v>
       </c>
       <c r="D220" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="I220" t="s">
         <v>674</v>
@@ -11248,7 +11656,7 @@
         <v>582</v>
       </c>
       <c r="D221" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="J221" s="2">
         <v>1</v>
@@ -11271,7 +11679,7 @@
         <v>583</v>
       </c>
       <c r="D222" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="J222" s="2">
         <v>1</v>
@@ -11317,7 +11725,7 @@
         <v>585</v>
       </c>
       <c r="D224" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="J224" s="2">
         <v>1</v>
@@ -11340,7 +11748,7 @@
         <v>586</v>
       </c>
       <c r="D225" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="J225" s="2">
         <v>1</v>
@@ -11363,7 +11771,7 @@
         <v>587</v>
       </c>
       <c r="D226" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="J226" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Debug missing variable name in crosswalk
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C495A6-1E7F-4620-B7B3-F6FE942713B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D1B09-8FB3-4D6D-89D9-25C71BEEF536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="1210">
   <si>
     <t>description</t>
   </si>
@@ -12097,9 +12097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8CABA-E2BC-451A-8F2B-D5B38142330D}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -12397,6 +12395,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>617</v>
+      </c>
       <c r="B25" s="7" t="s">
         <v>617</v>
       </c>

</xml_diff>

<commit_message>
Debug misspelt variable name in crosswalk
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D1B09-8FB3-4D6D-89D9-25C71BEEF536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E6902D-18AE-44C5-94C6-0E2F3B1A51FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
@@ -3678,7 +3678,7 @@
     <t>Q8.6</t>
   </si>
   <si>
-    <t>Bchaigender</t>
+    <t>BChairgender</t>
   </si>
 </sst>
 </file>
@@ -12097,7 +12097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8CABA-E2BC-451A-8F2B-D5B38142330D}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Add additional crosswalk columns
</commit_message>
<xml_diff>
--- a/dd-nptrends-wave-02.xlsx
+++ b/dd-nptrends-wave-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Urban\NCCS\nccs-nptrends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E6902D-18AE-44C5-94C6-0E2F3B1A51FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3A0610-D7C2-467B-A3B8-07BDF2F35346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="1210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="1213">
   <si>
     <t>description</t>
   </si>
@@ -3679,6 +3679,15 @@
   </si>
   <si>
     <t>BChairgender</t>
+  </si>
+  <si>
+    <t>Q8.2_4</t>
+  </si>
+  <si>
+    <t>Q8.2_5</t>
+  </si>
+  <si>
+    <t>Q8.2_6</t>
   </si>
 </sst>
 </file>
@@ -3749,7 +3758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3762,6 +3771,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4157,8 +4168,8 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C157" sqref="C157:C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12095,10 +12106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8CABA-E2BC-451A-8F2B-D5B38142330D}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12123,210 +12134,210 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>739</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1178</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>1179</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>1180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>740</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>1181</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>1182</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>1183</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>741</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>1184</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>1185</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>1186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>738</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
         <v>1187</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>1188</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>737</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>1190</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>765</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>1191</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>1193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>1194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="11" t="s">
         <v>728</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>1195</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>729</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>1196</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>730</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>1197</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>732</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>1198</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="11" t="s">
         <v>1009</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="8" t="s">
         <v>1199</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="8" t="s">
         <v>1200</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>1012</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="8" t="s">
         <v>1201</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="10" t="s">
         <v>752</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
         <v>1202</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>1203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="8" t="s">
         <v>1204</v>
       </c>
     </row>
@@ -12334,131 +12345,131 @@
       <c r="A18" t="s">
         <v>615</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>615</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
         <v>1205</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="10" t="s">
         <v>803</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="11" t="s">
         <v>804</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="10" t="s">
         <v>805</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="11" t="s">
         <v>806</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="10" t="s">
         <v>807</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="11" t="s">
         <v>808</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="10" t="s">
         <v>617</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
         <v>1206</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="11" t="s">
         <v>821</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="8" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="10" t="s">
         <v>822</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="8" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="11" t="s">
         <v>823</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="8" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="10" t="s">
         <v>824</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="8" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="11" t="s">
         <v>825</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="8" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="10" t="s">
         <v>826</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="8" t="s">
         <v>496</v>
       </c>
     </row>
@@ -12466,113 +12477,143 @@
       <c r="A32" t="s">
         <v>616</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>1207</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="11" t="s">
         <v>815</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="8" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="10" t="s">
         <v>816</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="8" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
         <v>817</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="8" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="10" t="s">
         <v>818</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="8" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="11" t="s">
         <v>819</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="8" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="10" t="s">
         <v>1209</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="8" t="s">
         <v>618</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7" t="s">
+      <c r="C38" s="8"/>
+      <c r="D38" s="9" t="s">
         <v>1208</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="10" t="s">
         <v>828</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="8" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="11" t="s">
         <v>829</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="8" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="10" t="s">
         <v>830</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="8" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="11" t="s">
         <v>831</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="8" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="10" t="s">
         <v>832</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="8" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C44" s="6"/>
+      <c r="A44" s="10" t="s">
+        <v>813</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>814</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>797</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1212</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>